<commit_message>
Basic functionality for data capture of IMU to matlab.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>GUID</t>
   </si>
@@ -402,6 +402,42 @@
   </si>
   <si>
     <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_ExpA1_006_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 22-Feb-2023 19:52:22</t>
+  </si>
+  <si>
+    <t>000061</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F1_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 25-Feb-2023 11:11:12</t>
+  </si>
+  <si>
+    <t>000062</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Accelerando_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F2_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 25-Feb-2023 11:11:22</t>
+  </si>
+  <si>
+    <t>000063</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Ritardando_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F3_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 25-Feb-2023 11:11:34</t>
+  </si>
+  <si>
+    <t>000064</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Lead in_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F4_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 25-Feb-2023 11:11:40</t>
+  </si>
+  <si>
+    <t>000065</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Cut off_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F5_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 25-Feb-2023 11:11:48</t>
+  </si>
+  <si>
+    <t>000066</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Crescendo_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F6_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 25-Feb-2023 11:12:00</t>
   </si>
 </sst>
 </file>
@@ -771,7 +807,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1271,6 +1307,54 @@
         <v>121</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Basic raw plot of accel gyro and magno, separately. READ for data capture updated with instructions.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>GUID</t>
   </si>
@@ -438,6 +438,36 @@
   </si>
   <si>
     <t>Details: 60bpm_mf_44path_Crescendo_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F6_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 25-Feb-2023 11:12:00</t>
+  </si>
+  <si>
+    <t>000067</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel, Gyro, and Magnometer data separately.. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:03:56</t>
+  </si>
+  <si>
+    <t>000068</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel, Gyro, and Magnometer data separately.. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:04:28</t>
+  </si>
+  <si>
+    <t>000069</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel, Gyro, and Magnometer data separately.. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:05:46</t>
+  </si>
+  <si>
+    <t>000070</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel, Gyro, and Magnometer data separately.. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:06:26</t>
+  </si>
+  <si>
+    <t>000071</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:07:03</t>
   </si>
 </sst>
 </file>
@@ -807,7 +837,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1355,6 +1385,46 @@
         <v>133</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
generated raw plots for accel and gyro readings, updated readme
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>GUID</t>
   </si>
@@ -468,6 +468,72 @@
   </si>
   <si>
     <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:07:03</t>
+  </si>
+  <si>
+    <t>000072</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:17:11</t>
+  </si>
+  <si>
+    <t>000073</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:17:30</t>
+  </si>
+  <si>
+    <t>000074</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:18:34</t>
+  </si>
+  <si>
+    <t>000075</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:18:48</t>
+  </si>
+  <si>
+    <t>000076</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:19:18</t>
+  </si>
+  <si>
+    <t>000077</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:19:45</t>
+  </si>
+  <si>
+    <t>000078</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:22:40</t>
+  </si>
+  <si>
+    <t>000079</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:22:58</t>
+  </si>
+  <si>
+    <t>000080</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:23:32</t>
+  </si>
+  <si>
+    <t>000081</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:23:57</t>
+  </si>
+  <si>
+    <t>000082</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:26:40</t>
   </si>
 </sst>
 </file>
@@ -837,7 +903,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1425,6 +1491,94 @@
         <v>143</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Baton tip pose from IMU orientation!
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>GUID</t>
   </si>
@@ -534,6 +534,30 @@
   </si>
   <si>
     <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 03-Mar-2023 10:26:40</t>
+  </si>
+  <si>
+    <t>000083</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 08-Mar-2023 10:28:53</t>
+  </si>
+  <si>
+    <t>000084</t>
+  </si>
+  <si>
+    <t>Details: IMU CJMCU-20948 Raw Data Reading - Raw Plots of 100 points of Accel Gyro and Magnometer data separately. Script used: Read_IMU.  Dataset used: Arduino Serial Output of IMU CJMCU-20948. File Location: Visualisations/IMU_RealRawData. Date Generated: 08-Mar-2023 10:29:27</t>
+  </si>
+  <si>
+    <t>000085</t>
+  </si>
+  <si>
+    <t>Details: Baton Tip Pose Transformation. IMU CJMCU-20948 Data Reading, Fused with imufilter, transformed with BatonTip_Transformation. Script used: BatonTipPoseVisualisation.  Dataset used: IMU data: IMU_Orientation_Reading_08_03_23. Transformed Baton tip data: BatonTipPose_08_03_23.. File Location: Visualisations/IMU_TransformedBatonTipPose. Date Generated: 08-Mar-2023 11:41:21</t>
+  </si>
+  <si>
+    <t>000086</t>
+  </si>
+  <si>
+    <t>Details: Baton Tip Pose Transformation. IMU CJMCU-20948 Data Reading, Fused with imufilter, transformed with BatonTip_Transformation. Script used: BatonTipPoseVisualisation.  Dataset used: IMU data: IMU_Orientation_Reading_08_03_23. Transformed Baton tip data: BatonTipPose_08_03_23.. File Location: Visualisations/IMU_TransformedBatonTipPose. Date Generated: 08-Mar-2023 11:44:01</t>
   </si>
 </sst>
 </file>
@@ -903,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -912,7 +936,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="341.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="348.7109375" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
@@ -1577,6 +1601,38 @@
       </c>
       <c r="B83" s="0" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
visualisation of baton tip transform and pose
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>GUID</t>
   </si>
@@ -558,6 +558,24 @@
   </si>
   <si>
     <t>Details: Baton Tip Pose Transformation. IMU CJMCU-20948 Data Reading, Fused with imufilter, transformed with BatonTip_Transformation. Script used: BatonTipPoseVisualisation.  Dataset used: IMU data: IMU_Orientation_Reading_08_03_23. Transformed Baton tip data: BatonTipPose_08_03_23.. File Location: Visualisations/IMU_TransformedBatonTipPose. Date Generated: 08-Mar-2023 11:44:01</t>
+  </si>
+  <si>
+    <t>000087</t>
+  </si>
+  <si>
+    <t>Details: Baton Tip Pose Transformation. IMU CJMCU-20948 Data Reading, Fused with imufilter, transformed with BatonTip_Transformation. Script used: BatonTipPoseVisualisation.  Dataset used: IMU data: IMU_Orientation_Reading_08_03_23. Transformed Baton tip data: BatonTipPose_08_03_23.. File Location: Visualisations/IMU_TransformedBatonTipPose. Date Generated: 08-Mar-2023 13:46:35</t>
+  </si>
+  <si>
+    <t>000088</t>
+  </si>
+  <si>
+    <t>Details: Baton Tip Pose Transformation - IMU CJMCU-20948 Data Reading, Fused with imufilter, transformed with BatonTip_Transformation. Script used: BatonTipPoseVisualisation.  Dataset used: IMU data: IMU_Orientation_Reading_08_03_23. Transformed Baton tip data: BatonTipPose_08_03_23.. File Location: Visualisations/IMU_TransformedBatonTipPose. Date Generated: 08-Mar-2023 13:46:56</t>
+  </si>
+  <si>
+    <t>000089</t>
+  </si>
+  <si>
+    <t>Details: Baton Tip Pose Transformation - IMU CJMCU-20948 Data Reading - Fused with imufilter - transformed with BatonTip_Transformation. Script used: BatonTipPoseVisualisation.  Dataset used: IMU data: IMU_Orientation_Reading_08_03_23. Transformed Baton tip data: BatonTipPose_08_03_23.. File Location: Visualisations/IMU_TransformedBatonTipPose. Date Generated: 08-Mar-2023 13:48:33</t>
   </si>
 </sst>
 </file>
@@ -927,7 +945,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B87"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -936,7 +954,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="348.7109375" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="350.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
@@ -1633,6 +1651,30 @@
       </c>
       <c r="B87" s="0" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made binary equal axis images of individual cycles.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="392">
   <si>
     <t>GUID</t>
   </si>
@@ -576,6 +576,642 @@
   </si>
   <si>
     <t>Details: Baton Tip Pose Transformation - IMU CJMCU-20948 Data Reading - Fused with imufilter - transformed with BatonTip_Transformation. Script used: BatonTipPoseVisualisation.  Dataset used: IMU data: IMU_Orientation_Reading_08_03_23. Transformed Baton tip data: BatonTipPose_08_03_23.. File Location: Visualisations/IMU_TransformedBatonTipPose. Date Generated: 08-Mar-2023 13:48:33</t>
+  </si>
+  <si>
+    <t>000090</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:40</t>
+  </si>
+  <si>
+    <t>000091</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:40</t>
+  </si>
+  <si>
+    <t>000092</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:40</t>
+  </si>
+  <si>
+    <t>000093</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:40</t>
+  </si>
+  <si>
+    <t>000094</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:41</t>
+  </si>
+  <si>
+    <t>000095</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:55</t>
+  </si>
+  <si>
+    <t>000096</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000097</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000098</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000099</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000100</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000101</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000102</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000103</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000104</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000105</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000106</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:56</t>
+  </si>
+  <si>
+    <t>000107</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:57</t>
+  </si>
+  <si>
+    <t>000108</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:57</t>
+  </si>
+  <si>
+    <t>000109</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:57</t>
+  </si>
+  <si>
+    <t>000110</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:57</t>
+  </si>
+  <si>
+    <t>000111</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:57</t>
+  </si>
+  <si>
+    <t>000112</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:57</t>
+  </si>
+  <si>
+    <t>000113</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:57</t>
+  </si>
+  <si>
+    <t>000114</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:25:57</t>
+  </si>
+  <si>
+    <t>000115</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:28</t>
+  </si>
+  <si>
+    <t>000116</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:28</t>
+  </si>
+  <si>
+    <t>000117</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:28</t>
+  </si>
+  <si>
+    <t>000118</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:28</t>
+  </si>
+  <si>
+    <t>000119</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:28</t>
+  </si>
+  <si>
+    <t>000120</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:28</t>
+  </si>
+  <si>
+    <t>000121</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:28</t>
+  </si>
+  <si>
+    <t>000122</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:28</t>
+  </si>
+  <si>
+    <t>000123</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000124</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000125</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000126</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000127</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000128</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000129</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000130</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000131</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000132</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000133</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000134</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:29</t>
+  </si>
+  <si>
+    <t>000135</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:56</t>
+  </si>
+  <si>
+    <t>000136</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:56</t>
+  </si>
+  <si>
+    <t>000137</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:56</t>
+  </si>
+  <si>
+    <t>000138</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:56</t>
+  </si>
+  <si>
+    <t>000139</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000140</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000141</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000142</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000143</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000144</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000145</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000146</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000147</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000148</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000149</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000150</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:57</t>
+  </si>
+  <si>
+    <t>000151</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:58</t>
+  </si>
+  <si>
+    <t>000152</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:58</t>
+  </si>
+  <si>
+    <t>000153</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:58</t>
+  </si>
+  <si>
+    <t>000154</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:26:58</t>
+  </si>
+  <si>
+    <t>000155</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:57</t>
+  </si>
+  <si>
+    <t>000156</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:57</t>
+  </si>
+  <si>
+    <t>000157</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000158</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000159</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000160</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000161</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000162</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000163</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000164</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000165</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000166</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000167</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:58</t>
+  </si>
+  <si>
+    <t>000168</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:59</t>
+  </si>
+  <si>
+    <t>000169</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:59</t>
+  </si>
+  <si>
+    <t>000170</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:59</t>
+  </si>
+  <si>
+    <t>000171</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:59</t>
+  </si>
+  <si>
+    <t>000172</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:59</t>
+  </si>
+  <si>
+    <t>000173</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:59</t>
+  </si>
+  <si>
+    <t>000174</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:28:59</t>
+  </si>
+  <si>
+    <t>000175</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000176</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000177</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000178</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000179</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000180</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000181</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000182</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000183</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000184</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000185</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:00</t>
+  </si>
+  <si>
+    <t>000186</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:01</t>
+  </si>
+  <si>
+    <t>000187</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:01</t>
+  </si>
+  <si>
+    <t>000188</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:01</t>
+  </si>
+  <si>
+    <t>000189</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:01</t>
+  </si>
+  <si>
+    <t>000190</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_1_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:01</t>
+  </si>
+  <si>
+    <t>000191</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_2_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:01</t>
+  </si>
+  <si>
+    <t>000192</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:01</t>
+  </si>
+  <si>
+    <t>000193</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_4_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:01</t>
+  </si>
+  <si>
+    <t>000194</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_5_Resampled.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:30:01</t>
+  </si>
+  <si>
+    <t>000195</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_All_Resampled_Average.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_All_Resampled_Average.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:33:36</t>
   </si>
 </sst>
 </file>
@@ -945,7 +1581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B196"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -954,7 +1590,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="350.42578125" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="402.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
@@ -1675,6 +2311,854 @@
       </c>
       <c r="B90" s="0" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B189" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B190" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B191" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B192" s="0" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="B193" s="0" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B194" s="0" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B196" s="0" t="s">
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed .mat.png from single cycle figure images
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="442">
   <si>
     <t>GUID</t>
   </si>
@@ -1212,6 +1212,156 @@
   </si>
   <si>
     <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_All_Resampled_Average.mat. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_All_Resampled_Average.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:33:36</t>
+  </si>
+  <si>
+    <t>000196</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_All_Resampled_Average.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:42:33</t>
+  </si>
+  <si>
+    <t>000197</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_All_Resampled_Average.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:43:24</t>
+  </si>
+  <si>
+    <t>000198</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_All_Resampled_Average.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:43:43</t>
+  </si>
+  <si>
+    <t>000199</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_All_Resampled_Average.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:43:59</t>
+  </si>
+  <si>
+    <t>000200</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_All_Resampled_Average. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_All_Resampled_Average.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:44:40</t>
+  </si>
+  <si>
+    <t>000201</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_1_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:13</t>
+  </si>
+  <si>
+    <t>000202</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_2_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000203</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000204</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_4_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000205</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_5_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000206</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_1_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000207</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_2_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000208</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000209</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_4_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000210</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_5_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000211</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_1_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000212</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_2_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000213</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:14</t>
+  </si>
+  <si>
+    <t>000214</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_4_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:15</t>
+  </si>
+  <si>
+    <t>000215</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_5_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:15</t>
+  </si>
+  <si>
+    <t>000216</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_1_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:15</t>
+  </si>
+  <si>
+    <t>000217</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_2_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:15</t>
+  </si>
+  <si>
+    <t>000218</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:15</t>
+  </si>
+  <si>
+    <t>000219</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_4_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:15</t>
+  </si>
+  <si>
+    <t>000220</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_5_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:15</t>
   </si>
 </sst>
 </file>
@@ -1581,7 +1731,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B196"/>
+  <dimension ref="A1:B221"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -3161,6 +3311,206 @@
         <v>391</v>
       </c>
     </row>
+    <row r="197">
+      <c r="A197" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B198" s="0" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="B203" s="0" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="B211" s="0" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="B216" s="0" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="B219" s="0" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="B220" s="0" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="B221" s="0" t="s">
+        <v>441</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Visualisation for IMU plus Leap data is labelled and saved with GUID. Good work.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="452">
   <si>
     <t>GUID</t>
   </si>
@@ -1362,6 +1362,36 @@
   </si>
   <si>
     <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_5_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 08-Mar-2023 21:45:15</t>
+  </si>
+  <si>
+    <t>000221</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 12-Mar-2023 17:19:36</t>
+  </si>
+  <si>
+    <t>000222</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 12-Mar-2023 17:20:31</t>
+  </si>
+  <si>
+    <t>000223</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 12-Mar-2023 17:24:16</t>
+  </si>
+  <si>
+    <t>000224</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 12-Mar-2023 17:30:13</t>
+  </si>
+  <si>
+    <t>000225</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 12-Mar-2023 17:30:59</t>
   </si>
 </sst>
 </file>
@@ -1731,7 +1761,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B221"/>
+  <dimension ref="A1:B226"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -3511,6 +3541,46 @@
         <v>441</v>
       </c>
     </row>
+    <row r="222">
+      <c r="A222" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="B222" s="0" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="B223" s="0" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="B224" s="0" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="B225" s="0" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="B226" s="0" t="s">
+        <v>451</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
transformations are now correct. sample rate included for correct imu readings. we have a product, kind of!
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="618">
   <si>
     <t>GUID</t>
   </si>
@@ -1392,6 +1392,504 @@
   </si>
   <si>
     <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 12-Mar-2023 17:30:59</t>
+  </si>
+  <si>
+    <t>000226</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 09:02:11</t>
+  </si>
+  <si>
+    <t>000227</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 09:46:06</t>
+  </si>
+  <si>
+    <t>000228</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 09:51:07</t>
+  </si>
+  <si>
+    <t>000229</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 09:56:16</t>
+  </si>
+  <si>
+    <t>000230</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 09:57:11</t>
+  </si>
+  <si>
+    <t>000231</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:00:37</t>
+  </si>
+  <si>
+    <t>000232</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:01:07</t>
+  </si>
+  <si>
+    <t>000233</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:01:44</t>
+  </si>
+  <si>
+    <t>000234</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:05:02</t>
+  </si>
+  <si>
+    <t>000235</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:06:34</t>
+  </si>
+  <si>
+    <t>000236</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:09:23</t>
+  </si>
+  <si>
+    <t>000237</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:12:22</t>
+  </si>
+  <si>
+    <t>000238</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:13:35</t>
+  </si>
+  <si>
+    <t>000239</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:14:45</t>
+  </si>
+  <si>
+    <t>000240</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:15:49</t>
+  </si>
+  <si>
+    <t>000241</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:16:48</t>
+  </si>
+  <si>
+    <t>000242</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:18:48</t>
+  </si>
+  <si>
+    <t>000243</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:19:41</t>
+  </si>
+  <si>
+    <t>000244</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:23:04</t>
+  </si>
+  <si>
+    <t>000245</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:23:38</t>
+  </si>
+  <si>
+    <t>000246</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:24:24</t>
+  </si>
+  <si>
+    <t>000247</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:25:51</t>
+  </si>
+  <si>
+    <t>000248</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:29:23</t>
+  </si>
+  <si>
+    <t>000249</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:49:35</t>
+  </si>
+  <si>
+    <t>000250</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along y axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:52:02</t>
+  </si>
+  <si>
+    <t>000251</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:57:34</t>
+  </si>
+  <si>
+    <t>000252</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:57:59</t>
+  </si>
+  <si>
+    <t>000253</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:58:14</t>
+  </si>
+  <si>
+    <t>000254</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:59:22</t>
+  </si>
+  <si>
+    <t>000255</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 10:59:39</t>
+  </si>
+  <si>
+    <t>000256</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 11:00:10</t>
+  </si>
+  <si>
+    <t>000257</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 11:00:28</t>
+  </si>
+  <si>
+    <t>000258</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 11:01:37</t>
+  </si>
+  <si>
+    <t>000259</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 11:02:22</t>
+  </si>
+  <si>
+    <t>000260</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 11:02:52</t>
+  </si>
+  <si>
+    <t>000261</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 11:03:39</t>
+  </si>
+  <si>
+    <t>000262</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 11:04:47</t>
+  </si>
+  <si>
+    <t>000263</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 11:07:26</t>
+  </si>
+  <si>
+    <t>000264</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F1_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 17-Mar-2023 13:25:24</t>
+  </si>
+  <si>
+    <t>000265</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F1_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 17-Mar-2023 13:26:12</t>
+  </si>
+  <si>
+    <t>000266</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F1_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 17-Mar-2023 13:33:52</t>
+  </si>
+  <si>
+    <t>000267</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F1_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 17-Mar-2023 13:34:22</t>
+  </si>
+  <si>
+    <t>000268</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F1_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 17-Mar-2023 13:35:52</t>
+  </si>
+  <si>
+    <t>000269</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F1_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 17-Mar-2023 13:41:12</t>
+  </si>
+  <si>
+    <t>000270</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 13:47:18</t>
+  </si>
+  <si>
+    <t>000271</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F1_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 17-Mar-2023 14:13:20</t>
+  </si>
+  <si>
+    <t>000272</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_AllHabits. Script used: BasicVisualisation_AllAtOnce_HeatMap_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_SimpleCentroidTrackingData\Session01_Exp_F1_001_GHI_BlanksRemoved_SimpleCentroid.csv. File Location: Visualisations/Session01_SimpleCentroid_Figures. Date Generated: 17-Mar-2023 14:16:19</t>
+  </si>
+  <si>
+    <t>000273</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:35:45</t>
+  </si>
+  <si>
+    <t>000274</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:36:38</t>
+  </si>
+  <si>
+    <t>000275</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:37:12</t>
+  </si>
+  <si>
+    <t>000276</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:40:00</t>
+  </si>
+  <si>
+    <t>000277</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:41:51</t>
+  </si>
+  <si>
+    <t>000278</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:47:30</t>
+  </si>
+  <si>
+    <t>000279</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:49:21</t>
+  </si>
+  <si>
+    <t>000280</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:51:02</t>
+  </si>
+  <si>
+    <t>000281</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:51:58</t>
+  </si>
+  <si>
+    <t>000282</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 14:53:33</t>
+  </si>
+  <si>
+    <t>000283</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 15:03:59</t>
+  </si>
+  <si>
+    <t>000284</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 15:49:33</t>
+  </si>
+  <si>
+    <t>000285</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 15:51:45</t>
+  </si>
+  <si>
+    <t>000286</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 15:53:50</t>
+  </si>
+  <si>
+    <t>000287</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 15:54:22</t>
+  </si>
+  <si>
+    <t>000288</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:08:19</t>
+  </si>
+  <si>
+    <t>000289</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:08:54</t>
+  </si>
+  <si>
+    <t>000290</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:09:13</t>
+  </si>
+  <si>
+    <t>000291</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:10:48</t>
+  </si>
+  <si>
+    <t>000292</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:11:00</t>
+  </si>
+  <si>
+    <t>000293</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:11:25</t>
+  </si>
+  <si>
+    <t>000294</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:14:32</t>
+  </si>
+  <si>
+    <t>000295</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:14:43</t>
+  </si>
+  <si>
+    <t>000296</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:15:35</t>
+  </si>
+  <si>
+    <t>000297</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:23:09</t>
+  </si>
+  <si>
+    <t>000298</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:28:52</t>
+  </si>
+  <si>
+    <t>000299</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:29:34</t>
+  </si>
+  <si>
+    <t>000300</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:29:44</t>
+  </si>
+  <si>
+    <t>000301</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:29:59</t>
+  </si>
+  <si>
+    <t>000302</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:31:28</t>
+  </si>
+  <si>
+    <t>000303</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:31:41</t>
+  </si>
+  <si>
+    <t>000304</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:32:18</t>
+  </si>
+  <si>
+    <t>000305</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:37:22</t>
+  </si>
+  <si>
+    <t>000306</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:37:54</t>
+  </si>
+  <si>
+    <t>000307</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:40:04</t>
+  </si>
+  <si>
+    <t>000308</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 17-Mar-2023 16:40:47</t>
   </si>
 </sst>
 </file>
@@ -1761,7 +2259,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B226"/>
+  <dimension ref="A1:B309"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -3581,6 +4079,670 @@
         <v>451</v>
       </c>
     </row>
+    <row r="227">
+      <c r="A227" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B229" s="0" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B231" s="0" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="B232" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="B233" s="0" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="B234" s="0" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="B235" s="0" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="B236" s="0" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="B237" s="0" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="B239" s="0" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="B240" s="0" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="B241" s="0" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="B242" s="0" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="B243" s="0" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="B244" s="0" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="B245" s="0" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="B246" s="0" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="B247" s="0" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="B248" s="0" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="B249" s="0" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="B250" s="0" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="B251" s="0" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B252" s="0" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B253" s="0" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="B254" s="0" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="B255" s="0" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="B256" s="0" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="B257" s="0" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="B258" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="B259" s="0" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="B260" s="0" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="B261" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="B262" s="0" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="B263" s="0" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="B264" s="0" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="B265" s="0" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="B266" s="0" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="B267" s="0" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="B268" s="0" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="B269" s="0" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="B270" s="0" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="B271" s="0" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="B272" s="0" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B273" s="0" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="B274" s="0" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="B275" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="B276" s="0" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="B277" s="0" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="0" t="s">
+        <v>554</v>
+      </c>
+      <c r="B278" s="0" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="B279" s="0" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="0" t="s">
+        <v>558</v>
+      </c>
+      <c r="B280" s="0" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="B281" s="0" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B282" s="0" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="B283" s="0" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="B284" s="0" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="B285" s="0" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="B286" s="0" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="0" t="s">
+        <v>572</v>
+      </c>
+      <c r="B287" s="0" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="B288" s="0" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="0" t="s">
+        <v>576</v>
+      </c>
+      <c r="B289" s="0" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="0" t="s">
+        <v>578</v>
+      </c>
+      <c r="B290" s="0" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="B291" s="0" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="B292" s="0" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="B293" s="0" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="B294" s="0" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="B295" s="0" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B296" s="0" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="B297" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="B298" s="0" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="0" t="s">
+        <v>596</v>
+      </c>
+      <c r="B299" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="0" t="s">
+        <v>598</v>
+      </c>
+      <c r="B300" s="0" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="B301" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="B302" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="0" t="s">
+        <v>604</v>
+      </c>
+      <c r="B303" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="B304" s="0" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="B305" s="0" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="B306" s="0" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="B307" s="0" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="B308" s="0" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="B309" s="0" t="s">
+        <v>617</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
wifi arduino now integrated in reading leap device + imu. small graph pops up at the end of the loop to show where time was spent
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="630">
   <si>
     <t>GUID</t>
   </si>
@@ -1902,6 +1902,30 @@
   </si>
   <si>
     <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 24-Mar-2023 14:18:45</t>
+  </si>
+  <si>
+    <t>000311</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-May-2023 16:46:41</t>
+  </si>
+  <si>
+    <t>000312</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-May-2023 17:02:54</t>
+  </si>
+  <si>
+    <t>000313</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-May-2023 17:04:14</t>
+  </si>
+  <si>
+    <t>000314</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-May-2023 17:05:24</t>
   </si>
 </sst>
 </file>
@@ -2271,7 +2295,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B311"/>
+  <dimension ref="A1:B315"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -4771,6 +4795,38 @@
         <v>621</v>
       </c>
     </row>
+    <row r="312">
+      <c r="A312" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="B312" s="0" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="B313" s="0" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="B314" s="0" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="0" t="s">
+        <v>628</v>
+      </c>
+      <c r="B315" s="0" t="s">
+        <v>629</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added basic data analysis with rigid registration and scaling. pretty cool.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="676">
   <si>
     <t>GUID</t>
   </si>
@@ -1926,6 +1926,144 @@
   </si>
   <si>
     <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-May-2023 17:05:24</t>
+  </si>
+  <si>
+    <t>000315</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_1_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:24</t>
+  </si>
+  <si>
+    <t>000316</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_2_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:25</t>
+  </si>
+  <si>
+    <t>000317</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:25</t>
+  </si>
+  <si>
+    <t>000318</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_4_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:25</t>
+  </si>
+  <si>
+    <t>000319</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_003_SavedCycle_5_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_003_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:25</t>
+  </si>
+  <si>
+    <t>000320</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_1_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:25</t>
+  </si>
+  <si>
+    <t>000321</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_2_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:25</t>
+  </si>
+  <si>
+    <t>000322</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:25</t>
+  </si>
+  <si>
+    <t>000323</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_4_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:25</t>
+  </si>
+  <si>
+    <t>000324</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_004_SavedCycle_5_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_004_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:25</t>
+  </si>
+  <si>
+    <t>000325</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_1_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000326</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_2_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000327</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000328</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_4_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000329</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_005_SavedCycle_5_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_005_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000330</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_1_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000331</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_2_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000332</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000333</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_4_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000334</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_ExpA1_006_SavedCycle_5_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 12-May-2023 15:27:26</t>
+  </si>
+  <si>
+    <t>000335</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: PcRegisterIcpTest.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 12-May-2023 22:15:23</t>
+  </si>
+  <si>
+    <t>000336</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: PcRegisterIcpTest.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 12-May-2023 22:16:24</t>
+  </si>
+  <si>
+    <t>000337</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: PcRegisterIcpTest.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 12-May-2023 22:16:28</t>
   </si>
 </sst>
 </file>
@@ -2295,7 +2433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B315"/>
+  <dimension ref="A1:B338"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -4827,6 +4965,190 @@
         <v>629</v>
       </c>
     </row>
+    <row r="316">
+      <c r="A316" s="0" t="s">
+        <v>630</v>
+      </c>
+      <c r="B316" s="0" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="0" t="s">
+        <v>632</v>
+      </c>
+      <c r="B317" s="0" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="0" t="s">
+        <v>634</v>
+      </c>
+      <c r="B318" s="0" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="B319" s="0" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="0" t="s">
+        <v>638</v>
+      </c>
+      <c r="B320" s="0" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="0" t="s">
+        <v>640</v>
+      </c>
+      <c r="B321" s="0" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="0" t="s">
+        <v>642</v>
+      </c>
+      <c r="B322" s="0" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="0" t="s">
+        <v>644</v>
+      </c>
+      <c r="B323" s="0" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="0" t="s">
+        <v>646</v>
+      </c>
+      <c r="B324" s="0" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="0" t="s">
+        <v>648</v>
+      </c>
+      <c r="B325" s="0" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="0" t="s">
+        <v>650</v>
+      </c>
+      <c r="B326" s="0" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="B327" s="0" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="0" t="s">
+        <v>654</v>
+      </c>
+      <c r="B328" s="0" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="B329" s="0" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="0" t="s">
+        <v>658</v>
+      </c>
+      <c r="B330" s="0" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="B331" s="0" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="B332" s="0" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="B333" s="0" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="0" t="s">
+        <v>666</v>
+      </c>
+      <c r="B334" s="0" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="B335" s="0" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="B336" s="0" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="B337" s="0" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="B338" s="0" t="s">
+        <v>675</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
arrays now circle shifted around to highest Y point. more analysis done on non A products
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="1028">
   <si>
     <t>GUID</t>
   </si>
@@ -2064,6 +2064,1062 @@
   </si>
   <si>
     <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: PcRegisterIcpTest.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 12-May-2023 22:16:28</t>
+  </si>
+  <si>
+    <t>000338</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:05:02</t>
+  </si>
+  <si>
+    <t>000339</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:06:02</t>
+  </si>
+  <si>
+    <t>000340</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_003_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_003_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:06:04</t>
+  </si>
+  <si>
+    <t>000341</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_004_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_004_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:06:08</t>
+  </si>
+  <si>
+    <t>000342</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_005_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_005_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:06:10</t>
+  </si>
+  <si>
+    <t>000343</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_006_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_006_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:06:13</t>
+  </si>
+  <si>
+    <t>000344</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:27:31</t>
+  </si>
+  <si>
+    <t>000345</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:27:46</t>
+  </si>
+  <si>
+    <t>000346</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_003_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_003_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:27:49</t>
+  </si>
+  <si>
+    <t>000347</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_004_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_004_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:27:52</t>
+  </si>
+  <si>
+    <t>000348</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_005_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_005_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:27:55</t>
+  </si>
+  <si>
+    <t>000349</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_006_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_006_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:27:57</t>
+  </si>
+  <si>
+    <t>000350</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A2_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A2_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:00</t>
+  </si>
+  <si>
+    <t>000351</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A3_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A3_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:02</t>
+  </si>
+  <si>
+    <t>000352</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A4_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A4_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:04</t>
+  </si>
+  <si>
+    <t>000353</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A5_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A5_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:05</t>
+  </si>
+  <si>
+    <t>000354</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A6_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A6_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:07</t>
+  </si>
+  <si>
+    <t>000355</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A7_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A7_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:08</t>
+  </si>
+  <si>
+    <t>000356</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A8_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A8_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:10</t>
+  </si>
+  <si>
+    <t>000357</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A9_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A9_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:13</t>
+  </si>
+  <si>
+    <t>000358</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_B1_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:14</t>
+  </si>
+  <si>
+    <t>000359</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B2_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_B2_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:16</t>
+  </si>
+  <si>
+    <t>000360</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B3_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_B3_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:18</t>
+  </si>
+  <si>
+    <t>000361</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B4_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_B4_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:20</t>
+  </si>
+  <si>
+    <t>000362</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B5_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_B5_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:21</t>
+  </si>
+  <si>
+    <t>000363</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B6_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_B6_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:24</t>
+  </si>
+  <si>
+    <t>000364</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B7_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_B7_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:26</t>
+  </si>
+  <si>
+    <t>000365</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B8_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_B8_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:28</t>
+  </si>
+  <si>
+    <t>000366</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B9_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_B9_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:30</t>
+  </si>
+  <si>
+    <t>000367</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_C1_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_C1_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:33</t>
+  </si>
+  <si>
+    <t>000368</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_C2_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_C2_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:35</t>
+  </si>
+  <si>
+    <t>000369</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_C3_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_C3_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:37</t>
+  </si>
+  <si>
+    <t>000370</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_C4_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_C4_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:38</t>
+  </si>
+  <si>
+    <t>000371</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_C5_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_C5_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:39</t>
+  </si>
+  <si>
+    <t>000372</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_C6_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_C6_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:41</t>
+  </si>
+  <si>
+    <t>000373</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_C7_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_C7_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:44</t>
+  </si>
+  <si>
+    <t>000374</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_C8_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_C8_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:45</t>
+  </si>
+  <si>
+    <t>000375</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_C9_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_C9_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:47</t>
+  </si>
+  <si>
+    <t>000376</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D1_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D1_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:49</t>
+  </si>
+  <si>
+    <t>000377</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D1_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D1_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:51</t>
+  </si>
+  <si>
+    <t>000378</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D2_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D2_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:53</t>
+  </si>
+  <si>
+    <t>000379</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D3_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D3_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:55</t>
+  </si>
+  <si>
+    <t>000380</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D4_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D4_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:56</t>
+  </si>
+  <si>
+    <t>000381</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D5_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D5_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:57</t>
+  </si>
+  <si>
+    <t>000382</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D6_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D6_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:28:59</t>
+  </si>
+  <si>
+    <t>000383</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D7_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D7_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:02</t>
+  </si>
+  <si>
+    <t>000384</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D8_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D8_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:03</t>
+  </si>
+  <si>
+    <t>000385</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_D9_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_D9_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:05</t>
+  </si>
+  <si>
+    <t>000386</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_E1_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_E1_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:07</t>
+  </si>
+  <si>
+    <t>000387</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_E2_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_E2_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:09</t>
+  </si>
+  <si>
+    <t>000388</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_E3_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_E3_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:11</t>
+  </si>
+  <si>
+    <t>000389</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_E4_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_E4_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:12</t>
+  </si>
+  <si>
+    <t>000390</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_E5_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_E5_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:13</t>
+  </si>
+  <si>
+    <t>000391</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_E6_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_E6_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:16</t>
+  </si>
+  <si>
+    <t>000392</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_E7_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_E7_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:18</t>
+  </si>
+  <si>
+    <t>000393</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_E8_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_E8_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:20</t>
+  </si>
+  <si>
+    <t>000394</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_E9_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_E9_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:22</t>
+  </si>
+  <si>
+    <t>000395</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_F1_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_F1_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:24</t>
+  </si>
+  <si>
+    <t>000396</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_F2_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_F2_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:26</t>
+  </si>
+  <si>
+    <t>000397</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_F3_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_F3_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:29</t>
+  </si>
+  <si>
+    <t>000398</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_F4_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_F4_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:30</t>
+  </si>
+  <si>
+    <t>000399</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_F5_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_F5_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:31</t>
+  </si>
+  <si>
+    <t>000400</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_F6_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_F6_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:34</t>
+  </si>
+  <si>
+    <t>000401</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_F7_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_F7_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:37</t>
+  </si>
+  <si>
+    <t>000402</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_F8_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_F8_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:39</t>
+  </si>
+  <si>
+    <t>000403</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_F9_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_F9_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:40</t>
+  </si>
+  <si>
+    <t>000404</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_Z1_001_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_Z1_001_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 13-May-2023 18:29:42</t>
+  </si>
+  <si>
+    <t>000405</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:06:08</t>
+  </si>
+  <si>
+    <t>000406</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:06:41</t>
+  </si>
+  <si>
+    <t>000407</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:07:02</t>
+  </si>
+  <si>
+    <t>000408</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:07:11</t>
+  </si>
+  <si>
+    <t>000409</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:07:23</t>
+  </si>
+  <si>
+    <t>000410</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:08:01</t>
+  </si>
+  <si>
+    <t>000411</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:08:07</t>
+  </si>
+  <si>
+    <t>000412</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:08:12</t>
+  </si>
+  <si>
+    <t>000413</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:08:25</t>
+  </si>
+  <si>
+    <t>000414</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:08:36</t>
+  </si>
+  <si>
+    <t>000415</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:08:42</t>
+  </si>
+  <si>
+    <t>000416</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:09:09</t>
+  </si>
+  <si>
+    <t>000417</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:09:30</t>
+  </si>
+  <si>
+    <t>000418</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:09:43</t>
+  </si>
+  <si>
+    <t>000419</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:09:48</t>
+  </si>
+  <si>
+    <t>000420</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:09:53</t>
+  </si>
+  <si>
+    <t>000421</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:10:00</t>
+  </si>
+  <si>
+    <t>000422</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:10:31</t>
+  </si>
+  <si>
+    <t>000423</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:10:42</t>
+  </si>
+  <si>
+    <t>000424</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:10:47</t>
+  </si>
+  <si>
+    <t>000425</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:10:58</t>
+  </si>
+  <si>
+    <t>000426</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:11:04</t>
+  </si>
+  <si>
+    <t>000427</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:11:07</t>
+  </si>
+  <si>
+    <t>000428</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:11:12</t>
+  </si>
+  <si>
+    <t>000429</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:11:17</t>
+  </si>
+  <si>
+    <t>000430</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:11:21</t>
+  </si>
+  <si>
+    <t>000431</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:11:30</t>
+  </si>
+  <si>
+    <t>000432</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:11:34</t>
+  </si>
+  <si>
+    <t>000433</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:11:48</t>
+  </si>
+  <si>
+    <t>000434</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:11:56</t>
+  </si>
+  <si>
+    <t>000435</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:12:00</t>
+  </si>
+  <si>
+    <t>000436</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:12:04</t>
+  </si>
+  <si>
+    <t>000437</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:12:10</t>
+  </si>
+  <si>
+    <t>000438</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:12:33</t>
+  </si>
+  <si>
+    <t>000439</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:12:37</t>
+  </si>
+  <si>
+    <t>000440</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:12:40</t>
+  </si>
+  <si>
+    <t>000441</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:12:46</t>
+  </si>
+  <si>
+    <t>000442</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:13:04</t>
+  </si>
+  <si>
+    <t>000443</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:13:28</t>
+  </si>
+  <si>
+    <t>000444</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:13:32</t>
+  </si>
+  <si>
+    <t>000445</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:13:36</t>
+  </si>
+  <si>
+    <t>000446</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:13:41</t>
+  </si>
+  <si>
+    <t>000447</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:13:46</t>
+  </si>
+  <si>
+    <t>000448</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:14:00</t>
+  </si>
+  <si>
+    <t>000449</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:14:06</t>
+  </si>
+  <si>
+    <t>000450</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:14:13</t>
+  </si>
+  <si>
+    <t>000451</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:14:30</t>
+  </si>
+  <si>
+    <t>000452</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:19:25</t>
+  </si>
+  <si>
+    <t>000453</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:19:54</t>
+  </si>
+  <si>
+    <t>000454</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:21:40</t>
+  </si>
+  <si>
+    <t>000455</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:22:20</t>
+  </si>
+  <si>
+    <t>000456</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:22:34</t>
+  </si>
+  <si>
+    <t>000457</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:23:30</t>
+  </si>
+  <si>
+    <t>000458</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:23:39</t>
+  </si>
+  <si>
+    <t>000459</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:23:57</t>
+  </si>
+  <si>
+    <t>000460</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:24:24</t>
+  </si>
+  <si>
+    <t>000461</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:24:55</t>
+  </si>
+  <si>
+    <t>000462</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:25:07</t>
+  </si>
+  <si>
+    <t>000463</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:26:02</t>
+  </si>
+  <si>
+    <t>000464</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:26:59</t>
+  </si>
+  <si>
+    <t>000465</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:27:27</t>
+  </si>
+  <si>
+    <t>000466</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:27:39</t>
+  </si>
+  <si>
+    <t>000467</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:27:44</t>
+  </si>
+  <si>
+    <t>000468</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_006_SavedCycle_4_Resampled. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:28:02</t>
+  </si>
+  <si>
+    <t>000469</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:41:02</t>
+  </si>
+  <si>
+    <t>000470</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:41:30</t>
+  </si>
+  <si>
+    <t>000471</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:41:38</t>
+  </si>
+  <si>
+    <t>000472</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:43:30</t>
+  </si>
+  <si>
+    <t>000473</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/ession01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:48:09</t>
+  </si>
+  <si>
+    <t>000474</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/ession01_ExpA1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:48:48</t>
+  </si>
+  <si>
+    <t>000475</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/ession01 ExpA1 006 SavedCycle 4 Resampled.mat. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:49:01</t>
+  </si>
+  <si>
+    <t>000476</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle 4 Resampled.mat. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:49:09</t>
+  </si>
+  <si>
+    <t>000477</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:49:48</t>
+  </si>
+  <si>
+    <t>000478</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle 4 Res. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:50:27</t>
+  </si>
+  <si>
+    <t>000479</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle . File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:50:37</t>
+  </si>
+  <si>
+    <t>000480</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:50:44</t>
+  </si>
+  <si>
+    <t>000481</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:51:27</t>
+  </si>
+  <si>
+    <t>000482</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:51:39</t>
+  </si>
+  <si>
+    <t>000483</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:52:51</t>
+  </si>
+  <si>
+    <t>000484</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:53:04</t>
+  </si>
+  <si>
+    <t>000485</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:53:13</t>
+  </si>
+  <si>
+    <t>000486</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 ExpA1 006 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:56:08</t>
+  </si>
+  <si>
+    <t>000487</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/ession01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:57:00</t>
+  </si>
+  <si>
+    <t>000488</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/ession01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:57:23</t>
+  </si>
+  <si>
+    <t>000489</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:58:02</t>
+  </si>
+  <si>
+    <t>000490</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 19:58:47</t>
+  </si>
+  <si>
+    <t>000491</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:02:20</t>
+  </si>
+  <si>
+    <t>000492</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 003 SavedCycle 5. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:02:36</t>
+  </si>
+  <si>
+    <t>000493</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 004 SavedCycle 5. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:02:43</t>
+  </si>
+  <si>
+    <t>000494</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 004 SavedCycle 5. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:03:07</t>
+  </si>
+  <si>
+    <t>000495</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:03:14</t>
+  </si>
+  <si>
+    <t>000496</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:03:23</t>
+  </si>
+  <si>
+    <t>000497</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:03:27</t>
+  </si>
+  <si>
+    <t>000498</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:03:40</t>
+  </si>
+  <si>
+    <t>000499</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:03:51</t>
+  </si>
+  <si>
+    <t>000500</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:04:04</t>
+  </si>
+  <si>
+    <t>000501</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:05:31</t>
+  </si>
+  <si>
+    <t>000502</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F9 001 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:05:36</t>
+  </si>
+  <si>
+    <t>000503</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F9 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:05:48</t>
+  </si>
+  <si>
+    <t>000504</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F9 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:05:56</t>
+  </si>
+  <si>
+    <t>000505</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F7 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:06:11</t>
+  </si>
+  <si>
+    <t>000506</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F7 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:06:28</t>
+  </si>
+  <si>
+    <t>000507</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F7 001 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:06:32</t>
+  </si>
+  <si>
+    <t>000508</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F7 001 SavedCycle 5. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:06:38</t>
+  </si>
+  <si>
+    <t>000509</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F7 001 SavedCycle 5. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:08:04</t>
+  </si>
+  <si>
+    <t>000510</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:08:19</t>
+  </si>
+  <si>
+    <t>000511</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E9 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:09:25</t>
+  </si>
+  <si>
+    <t>000512</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 004 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:09:46</t>
+  </si>
+  <si>
+    <t>000513</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:10:44</t>
   </si>
 </sst>
 </file>
@@ -2433,7 +3489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B338"/>
+  <dimension ref="A1:B514"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -2442,7 +3498,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="402.42578125" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="557.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
@@ -5147,6 +6203,1414 @@
       </c>
       <c r="B338" s="0" t="s">
         <v>675</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="B339" s="0" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="0" t="s">
+        <v>678</v>
+      </c>
+      <c r="B340" s="0" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="B341" s="0" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="B342" s="0" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="B343" s="0" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="B344" s="0" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="B345" s="0" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B346" s="0" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="B347" s="0" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="0" t="s">
+        <v>694</v>
+      </c>
+      <c r="B348" s="0" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="B349" s="0" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="B350" s="0" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="0" t="s">
+        <v>700</v>
+      </c>
+      <c r="B351" s="0" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="B352" s="0" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="B353" s="0" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="B354" s="0" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="0" t="s">
+        <v>708</v>
+      </c>
+      <c r="B355" s="0" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="B356" s="0" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="B357" s="0" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="B358" s="0" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="0" t="s">
+        <v>716</v>
+      </c>
+      <c r="B359" s="0" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="0" t="s">
+        <v>718</v>
+      </c>
+      <c r="B360" s="0" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="0" t="s">
+        <v>720</v>
+      </c>
+      <c r="B361" s="0" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="B362" s="0" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="0" t="s">
+        <v>724</v>
+      </c>
+      <c r="B363" s="0" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B364" s="0" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="0" t="s">
+        <v>728</v>
+      </c>
+      <c r="B365" s="0" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="0" t="s">
+        <v>730</v>
+      </c>
+      <c r="B366" s="0" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="0" t="s">
+        <v>732</v>
+      </c>
+      <c r="B367" s="0" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="0" t="s">
+        <v>734</v>
+      </c>
+      <c r="B368" s="0" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="0" t="s">
+        <v>736</v>
+      </c>
+      <c r="B369" s="0" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="0" t="s">
+        <v>738</v>
+      </c>
+      <c r="B370" s="0" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="B371" s="0" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="0" t="s">
+        <v>742</v>
+      </c>
+      <c r="B372" s="0" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="B373" s="0" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="0" t="s">
+        <v>746</v>
+      </c>
+      <c r="B374" s="0" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="0" t="s">
+        <v>748</v>
+      </c>
+      <c r="B375" s="0" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="0" t="s">
+        <v>750</v>
+      </c>
+      <c r="B376" s="0" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="B377" s="0" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="0" t="s">
+        <v>754</v>
+      </c>
+      <c r="B378" s="0" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="0" t="s">
+        <v>756</v>
+      </c>
+      <c r="B379" s="0" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="0" t="s">
+        <v>758</v>
+      </c>
+      <c r="B380" s="0" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="0" t="s">
+        <v>760</v>
+      </c>
+      <c r="B381" s="0" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="0" t="s">
+        <v>762</v>
+      </c>
+      <c r="B382" s="0" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="B383" s="0" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="0" t="s">
+        <v>766</v>
+      </c>
+      <c r="B384" s="0" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="B385" s="0" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="0" t="s">
+        <v>770</v>
+      </c>
+      <c r="B386" s="0" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="0" t="s">
+        <v>772</v>
+      </c>
+      <c r="B387" s="0" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="0" t="s">
+        <v>774</v>
+      </c>
+      <c r="B388" s="0" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="0" t="s">
+        <v>776</v>
+      </c>
+      <c r="B389" s="0" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="0" t="s">
+        <v>778</v>
+      </c>
+      <c r="B390" s="0" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B391" s="0" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="0" t="s">
+        <v>782</v>
+      </c>
+      <c r="B392" s="0" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="0" t="s">
+        <v>784</v>
+      </c>
+      <c r="B393" s="0" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="0" t="s">
+        <v>786</v>
+      </c>
+      <c r="B394" s="0" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="0" t="s">
+        <v>788</v>
+      </c>
+      <c r="B395" s="0" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="0" t="s">
+        <v>790</v>
+      </c>
+      <c r="B396" s="0" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="0" t="s">
+        <v>792</v>
+      </c>
+      <c r="B397" s="0" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="B398" s="0" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="0" t="s">
+        <v>796</v>
+      </c>
+      <c r="B399" s="0" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="0" t="s">
+        <v>798</v>
+      </c>
+      <c r="B400" s="0" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="0" t="s">
+        <v>800</v>
+      </c>
+      <c r="B401" s="0" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="B402" s="0" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="B403" s="0" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="0" t="s">
+        <v>806</v>
+      </c>
+      <c r="B404" s="0" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="0" t="s">
+        <v>808</v>
+      </c>
+      <c r="B405" s="0" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="B406" s="0" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="0" t="s">
+        <v>812</v>
+      </c>
+      <c r="B407" s="0" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="0" t="s">
+        <v>814</v>
+      </c>
+      <c r="B408" s="0" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="0" t="s">
+        <v>816</v>
+      </c>
+      <c r="B409" s="0" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="0" t="s">
+        <v>818</v>
+      </c>
+      <c r="B410" s="0" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="B411" s="0" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="0" t="s">
+        <v>822</v>
+      </c>
+      <c r="B412" s="0" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="0" t="s">
+        <v>824</v>
+      </c>
+      <c r="B413" s="0" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="B414" s="0" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="0" t="s">
+        <v>828</v>
+      </c>
+      <c r="B415" s="0" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="B416" s="0" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="0" t="s">
+        <v>832</v>
+      </c>
+      <c r="B417" s="0" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="0" t="s">
+        <v>834</v>
+      </c>
+      <c r="B418" s="0" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="B419" s="0" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="B420" s="0" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="B421" s="0" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="0" t="s">
+        <v>842</v>
+      </c>
+      <c r="B422" s="0" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="B423" s="0" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="0" t="s">
+        <v>846</v>
+      </c>
+      <c r="B424" s="0" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="0" t="s">
+        <v>848</v>
+      </c>
+      <c r="B425" s="0" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="0" t="s">
+        <v>850</v>
+      </c>
+      <c r="B426" s="0" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="B427" s="0" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="B428" s="0" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="B429" s="0" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="B430" s="0" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="0" t="s">
+        <v>860</v>
+      </c>
+      <c r="B431" s="0" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="B432" s="0" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="0" t="s">
+        <v>864</v>
+      </c>
+      <c r="B433" s="0" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="0" t="s">
+        <v>866</v>
+      </c>
+      <c r="B434" s="0" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="B435" s="0" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="0" t="s">
+        <v>870</v>
+      </c>
+      <c r="B436" s="0" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="B437" s="0" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="0" t="s">
+        <v>874</v>
+      </c>
+      <c r="B438" s="0" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="0" t="s">
+        <v>876</v>
+      </c>
+      <c r="B439" s="0" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="0" t="s">
+        <v>878</v>
+      </c>
+      <c r="B440" s="0" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="0" t="s">
+        <v>880</v>
+      </c>
+      <c r="B441" s="0" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="0" t="s">
+        <v>882</v>
+      </c>
+      <c r="B442" s="0" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="0" t="s">
+        <v>884</v>
+      </c>
+      <c r="B443" s="0" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="0" t="s">
+        <v>886</v>
+      </c>
+      <c r="B444" s="0" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="0" t="s">
+        <v>888</v>
+      </c>
+      <c r="B445" s="0" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="0" t="s">
+        <v>890</v>
+      </c>
+      <c r="B446" s="0" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="0" t="s">
+        <v>892</v>
+      </c>
+      <c r="B447" s="0" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="0" t="s">
+        <v>894</v>
+      </c>
+      <c r="B448" s="0" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="0" t="s">
+        <v>896</v>
+      </c>
+      <c r="B449" s="0" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="0" t="s">
+        <v>898</v>
+      </c>
+      <c r="B450" s="0" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="0" t="s">
+        <v>900</v>
+      </c>
+      <c r="B451" s="0" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="0" t="s">
+        <v>902</v>
+      </c>
+      <c r="B452" s="0" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="0" t="s">
+        <v>904</v>
+      </c>
+      <c r="B453" s="0" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="0" t="s">
+        <v>906</v>
+      </c>
+      <c r="B454" s="0" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="0" t="s">
+        <v>908</v>
+      </c>
+      <c r="B455" s="0" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="0" t="s">
+        <v>910</v>
+      </c>
+      <c r="B456" s="0" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="0" t="s">
+        <v>912</v>
+      </c>
+      <c r="B457" s="0" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="B458" s="0" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="0" t="s">
+        <v>916</v>
+      </c>
+      <c r="B459" s="0" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="0" t="s">
+        <v>918</v>
+      </c>
+      <c r="B460" s="0" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="0" t="s">
+        <v>920</v>
+      </c>
+      <c r="B461" s="0" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="B462" s="0" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="0" t="s">
+        <v>924</v>
+      </c>
+      <c r="B463" s="0" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="0" t="s">
+        <v>926</v>
+      </c>
+      <c r="B464" s="0" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="0" t="s">
+        <v>928</v>
+      </c>
+      <c r="B465" s="0" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="0" t="s">
+        <v>930</v>
+      </c>
+      <c r="B466" s="0" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="0" t="s">
+        <v>932</v>
+      </c>
+      <c r="B467" s="0" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="0" t="s">
+        <v>934</v>
+      </c>
+      <c r="B468" s="0" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="0" t="s">
+        <v>936</v>
+      </c>
+      <c r="B469" s="0" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="0" t="s">
+        <v>938</v>
+      </c>
+      <c r="B470" s="0" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="B471" s="0" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="0" t="s">
+        <v>942</v>
+      </c>
+      <c r="B472" s="0" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B473" s="0" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="0" t="s">
+        <v>946</v>
+      </c>
+      <c r="B474" s="0" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="0" t="s">
+        <v>948</v>
+      </c>
+      <c r="B475" s="0" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="0" t="s">
+        <v>950</v>
+      </c>
+      <c r="B476" s="0" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="0" t="s">
+        <v>952</v>
+      </c>
+      <c r="B477" s="0" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="0" t="s">
+        <v>954</v>
+      </c>
+      <c r="B478" s="0" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="0" t="s">
+        <v>956</v>
+      </c>
+      <c r="B479" s="0" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="0" t="s">
+        <v>958</v>
+      </c>
+      <c r="B480" s="0" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="0" t="s">
+        <v>960</v>
+      </c>
+      <c r="B481" s="0" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="0" t="s">
+        <v>962</v>
+      </c>
+      <c r="B482" s="0" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="0" t="s">
+        <v>964</v>
+      </c>
+      <c r="B483" s="0" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="0" t="s">
+        <v>966</v>
+      </c>
+      <c r="B484" s="0" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="B485" s="0" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="0" t="s">
+        <v>970</v>
+      </c>
+      <c r="B486" s="0" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="0" t="s">
+        <v>972</v>
+      </c>
+      <c r="B487" s="0" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="0" t="s">
+        <v>974</v>
+      </c>
+      <c r="B488" s="0" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="0" t="s">
+        <v>976</v>
+      </c>
+      <c r="B489" s="0" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="0" t="s">
+        <v>978</v>
+      </c>
+      <c r="B490" s="0" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="0" t="s">
+        <v>980</v>
+      </c>
+      <c r="B491" s="0" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="B492" s="0" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="0" t="s">
+        <v>984</v>
+      </c>
+      <c r="B493" s="0" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="0" t="s">
+        <v>986</v>
+      </c>
+      <c r="B494" s="0" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="0" t="s">
+        <v>988</v>
+      </c>
+      <c r="B495" s="0" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="0" t="s">
+        <v>990</v>
+      </c>
+      <c r="B496" s="0" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="0" t="s">
+        <v>992</v>
+      </c>
+      <c r="B497" s="0" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="0" t="s">
+        <v>994</v>
+      </c>
+      <c r="B498" s="0" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="0" t="s">
+        <v>996</v>
+      </c>
+      <c r="B499" s="0" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="0" t="s">
+        <v>998</v>
+      </c>
+      <c r="B500" s="0" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="0" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B501" s="0" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="0" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B502" s="0" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="0" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B503" s="0" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="0" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B504" s="0" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="0" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B505" s="0" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="0" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B506" s="0" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="0" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B507" s="0" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="0" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B508" s="0" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="0" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B509" s="0" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="0" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B510" s="0" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="0" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B511" s="0" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="0" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B512" s="0" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="0" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B513" s="0" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="0" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B514" s="0" t="s">
+        <v>1027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back to serial input for the IMU. faded colour added for clarity of plot. only plotting non zero values within arrays (partially working). unhappy with the difference seen in the baton tip and palm, cannot see the differences in wrist that we saw in optitrack.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="1034">
   <si>
     <t>GUID</t>
   </si>
@@ -3120,6 +3120,24 @@
   </si>
   <si>
     <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: HalfRigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 13-May-2023 20:10:44</t>
+  </si>
+  <si>
+    <t>000514</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 01-Jun-2023 16:18:30</t>
+  </si>
+  <si>
+    <t>000515</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 01-Jun-2023 17:16:22</t>
+  </si>
+  <si>
+    <t>000516</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 01-Jun-2023 17:35:54</t>
   </si>
 </sst>
 </file>
@@ -3489,7 +3507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B514"/>
+  <dimension ref="A1:B517"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -7613,6 +7631,30 @@
         <v>1027</v>
       </c>
     </row>
+    <row r="515">
+      <c r="A515" s="0" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B515" s="0" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="0" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B516" s="0" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="0" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B517" s="0" t="s">
+        <v>1033</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
averages for all movement types calculated. inidividual movements compared to all movement types.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="1144">
   <si>
     <t>GUID</t>
   </si>
@@ -3138,6 +3138,336 @@
   </si>
   <si>
     <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 01-Jun-2023 17:35:54</t>
+  </si>
+  <si>
+    <t>000517</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_1_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_1_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 07-Jun-2023 12:59:42</t>
+  </si>
+  <si>
+    <t>000518</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_2_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 07-Jun-2023 12:59:43</t>
+  </si>
+  <si>
+    <t>000519</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 07-Jun-2023 12:59:43</t>
+  </si>
+  <si>
+    <t>000520</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:03:58</t>
+  </si>
+  <si>
+    <t>000521</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:04:14</t>
+  </si>
+  <si>
+    <t>000522</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:04:29</t>
+  </si>
+  <si>
+    <t>000523</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:04:33</t>
+  </si>
+  <si>
+    <t>000524</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:04:39</t>
+  </si>
+  <si>
+    <t>000525</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:06:03</t>
+  </si>
+  <si>
+    <t>000526</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:06:07</t>
+  </si>
+  <si>
+    <t>000527</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:15:50</t>
+  </si>
+  <si>
+    <t>000528</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:16:08</t>
+  </si>
+  <si>
+    <t>000529</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:16:18</t>
+  </si>
+  <si>
+    <t>000530</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:17:17</t>
+  </si>
+  <si>
+    <t>000531</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. Script used: ResampledVisualisationCycles_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:17:37</t>
+  </si>
+  <si>
+    <t>000532</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Waist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_C1_001_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:19:07</t>
+  </si>
+  <si>
+    <t>000533</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Knees. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_B1_001_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:20:25</t>
+  </si>
+  <si>
+    <t>000534</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Knees. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:26:39</t>
+  </si>
+  <si>
+    <t>000535</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Knees. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:26:54</t>
+  </si>
+  <si>
+    <t>000536</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:27:04</t>
+  </si>
+  <si>
+    <t>000537</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_E1_001_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:27:49</t>
+  </si>
+  <si>
+    <t>000538</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Wrist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_E1_001_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:28:11</t>
+  </si>
+  <si>
+    <t>000539</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Wrist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_E1_001_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:28:54</t>
+  </si>
+  <si>
+    <t>000540</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_2_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 07-Jun-2023 13:29:05</t>
+  </si>
+  <si>
+    <t>000541</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 13:30:07</t>
+  </si>
+  <si>
+    <t>000542</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 13:58:56</t>
+  </si>
+  <si>
+    <t>000543</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 13:59:38</t>
+  </si>
+  <si>
+    <t>000544</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:03:29</t>
+  </si>
+  <si>
+    <t>000545</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:04:08</t>
+  </si>
+  <si>
+    <t>000546</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:04:57</t>
+  </si>
+  <si>
+    <t>000547</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:07:46</t>
+  </si>
+  <si>
+    <t>000548</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:08:27</t>
+  </si>
+  <si>
+    <t>000549</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:08:49</t>
+  </si>
+  <si>
+    <t>000550</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:10:47</t>
+  </si>
+  <si>
+    <t>000551</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:12:27</t>
+  </si>
+  <si>
+    <t>000552</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:19:36</t>
+  </si>
+  <si>
+    <t>000553</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:19:56</t>
+  </si>
+  <si>
+    <t>000554</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:20:22</t>
+  </si>
+  <si>
+    <t>000555</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:20:36</t>
+  </si>
+  <si>
+    <t>000556</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:20:48</t>
+  </si>
+  <si>
+    <t>000557</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:21:35</t>
+  </si>
+  <si>
+    <t>000558</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:21:54</t>
+  </si>
+  <si>
+    <t>000559</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:29:09</t>
+  </si>
+  <si>
+    <t>000560</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:30:03</t>
+  </si>
+  <si>
+    <t>000561</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:31:52</t>
+  </si>
+  <si>
+    <t>000562</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:32:07</t>
+  </si>
+  <si>
+    <t>000563</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:32:55</t>
+  </si>
+  <si>
+    <t>000564</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:33:37</t>
+  </si>
+  <si>
+    <t>000565</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:33:51</t>
+  </si>
+  <si>
+    <t>000566</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:34:23</t>
+  </si>
+  <si>
+    <t>000567</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:34:53</t>
+  </si>
+  <si>
+    <t>000568</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 003 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:36:23</t>
+  </si>
+  <si>
+    <t>000569</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 003 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:36:30</t>
+  </si>
+  <si>
+    <t>000570</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:36:37</t>
+  </si>
+  <si>
+    <t>000571</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:37:35</t>
   </si>
 </sst>
 </file>
@@ -3507,7 +3837,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B517"/>
+  <dimension ref="A1:B572"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -7655,6 +7985,446 @@
         <v>1033</v>
       </c>
     </row>
+    <row r="518">
+      <c r="A518" s="0" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B518" s="0" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="0" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B519" s="0" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="0" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B520" s="0" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="0" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B521" s="0" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="0" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B522" s="0" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="0" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B523" s="0" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="0" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B524" s="0" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="0" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B525" s="0" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="0" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B526" s="0" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="0" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B527" s="0" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="0" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B528" s="0" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B529" s="0" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="0" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B530" s="0" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="0" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B531" s="0" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="0" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B532" s="0" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="0" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B533" s="0" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="0" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B534" s="0" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="0" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B535" s="0" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="0" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B536" s="0" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="0" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B537" s="0" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="0" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B538" s="0" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="0" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B539" s="0" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="0" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B540" s="0" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="0" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B541" s="0" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="0" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B542" s="0" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="0" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B543" s="0" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="0" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B544" s="0" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="0" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B545" s="0" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="0" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B546" s="0" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="0" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B547" s="0" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="0" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B548" s="0" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B549" s="0" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="0" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B550" s="0" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="0" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B551" s="0" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="0" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B552" s="0" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B553" s="0" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="0" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B554" s="0" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B555" s="0" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="0" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B556" s="0" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="0" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B557" s="0" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B558" s="0" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B559" s="0" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="0" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B560" s="0" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="0" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B561" s="0" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="0" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B562" s="0" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="0" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B563" s="0" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="0" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B564" s="0" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B565" s="0" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="0" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B566" s="0" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B567" s="0" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B568" s="0" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B569" s="0" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="0" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B570" s="0" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B571" s="0" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="0" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B572" s="0" t="s">
+        <v>1143</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Resampled and scaled Session02 motive data to be the same size and number of points as session02 leap data. interpreted results to plot overlaid. motive data is wrong orientation.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="1200">
   <si>
     <t>GUID</t>
   </si>
@@ -3468,6 +3468,174 @@
   </si>
   <si>
     <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 07-Jun-2023 14:37:35</t>
+  </si>
+  <si>
+    <t>000572</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 16:29:24</t>
+  </si>
+  <si>
+    <t>000573</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 16:31:04</t>
+  </si>
+  <si>
+    <t>000573</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 16:31:51</t>
+  </si>
+  <si>
+    <t>000574</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 16:34:48</t>
+  </si>
+  <si>
+    <t>000575</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 16:35:53</t>
+  </si>
+  <si>
+    <t>000576</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 16:36:19</t>
+  </si>
+  <si>
+    <t>000577</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:44:45</t>
+  </si>
+  <si>
+    <t>000578</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:45:09</t>
+  </si>
+  <si>
+    <t>000579</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:46:04</t>
+  </si>
+  <si>
+    <t>000580</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:49:36</t>
+  </si>
+  <si>
+    <t>000581</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:49:49</t>
+  </si>
+  <si>
+    <t>000582</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:50:16</t>
+  </si>
+  <si>
+    <t>000583</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:50:42</t>
+  </si>
+  <si>
+    <t>000584</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:51:13</t>
+  </si>
+  <si>
+    <t>000585</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:51:32</t>
+  </si>
+  <si>
+    <t>000586</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:52:51</t>
+  </si>
+  <si>
+    <t>000587</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 17:54:50</t>
+  </si>
+  <si>
+    <t>000588</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 18:00:21</t>
+  </si>
+  <si>
+    <t>000589</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 09-Jun-2023 18:01:09</t>
+  </si>
+  <si>
+    <t>000590</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 10-Jun-2023 09:17:29</t>
+  </si>
+  <si>
+    <t>000591</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 13:43:15</t>
+  </si>
+  <si>
+    <t>000592</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 13:44:00</t>
+  </si>
+  <si>
+    <t>000593</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 41B. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 13:47:27</t>
+  </si>
+  <si>
+    <t>000594</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 32B. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 13:47:50</t>
+  </si>
+  <si>
+    <t>000595</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 32B. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 13:48:14</t>
+  </si>
+  <si>
+    <t>000596</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 22B. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 13:49:27</t>
+  </si>
+  <si>
+    <t>000597</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 42E. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 13:50:14</t>
+  </si>
+  <si>
+    <t>000598</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 42E. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 13:50:43</t>
   </si>
 </sst>
 </file>
@@ -3837,7 +4005,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B572"/>
+  <dimension ref="A1:B600"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -8425,6 +8593,230 @@
         <v>1143</v>
       </c>
     </row>
+    <row r="573">
+      <c r="A573" s="0" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B573" s="0" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="0" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B574" s="0" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="0" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B575" s="0" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B576" s="0" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="0" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B577" s="0" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B578" s="0" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="0" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B579" s="0" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="0" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B580" s="0" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" s="0" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B581" s="0" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B582" s="0" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B583" s="0" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B584" s="0" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="0" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B585" s="0" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="0" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B586" s="0" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" s="0" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B587" s="0" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" s="0" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B588" s="0" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" s="0" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B589" s="0" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B590" s="0" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B591" s="0" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" s="0" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B592" s="0" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B593" s="0" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" s="0" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B594" s="0" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B595" s="0" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B596" s="0" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B597" s="0" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" s="0" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B598" s="0" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B599" s="0" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" s="0" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B600" s="0" t="s">
+        <v>1199</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added motive rotation, although some datasets seem to need it while others don't. fixed the 000 point showing up, the first and last indexes of palm and smooth baton were mixed up.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="1200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="1228">
   <si>
     <t>GUID</t>
   </si>
@@ -3636,6 +3636,90 @@
   </si>
   <si>
     <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 42E. Script used: Interpret_IMU_And_LeapDevice_And_Motive.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 13:50:43</t>
+  </si>
+  <si>
+    <t>000599</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 13B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:28:16</t>
+  </si>
+  <si>
+    <t>000600</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 13B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:28:49</t>
+  </si>
+  <si>
+    <t>000601</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 14B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:29:07</t>
+  </si>
+  <si>
+    <t>000602</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 14C. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:29:23</t>
+  </si>
+  <si>
+    <t>000603</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:29:43</t>
+  </si>
+  <si>
+    <t>000604</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 22B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:30:05</t>
+  </si>
+  <si>
+    <t>000605</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 23B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:30:22</t>
+  </si>
+  <si>
+    <t>000606</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:31:28</t>
+  </si>
+  <si>
+    <t>000607</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:32:19</t>
+  </si>
+  <si>
+    <t>000608</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:33:32</t>
+  </si>
+  <si>
+    <t>000609</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:34:01</t>
+  </si>
+  <si>
+    <t>000610</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:35:12</t>
+  </si>
+  <si>
+    <t>000611</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:38:12</t>
+  </si>
+  <si>
+    <t>000612</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:38:57</t>
   </si>
 </sst>
 </file>
@@ -4005,7 +4089,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B600"/>
+  <dimension ref="A1:B614"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -8817,6 +8901,118 @@
         <v>1199</v>
       </c>
     </row>
+    <row r="601">
+      <c r="A601" s="0" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B601" s="0" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" s="0" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B602" s="0" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" s="0" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B603" s="0" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B604" s="0" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" s="0" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B605" s="0" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" s="0" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B606" s="0" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" s="0" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B607" s="0" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" s="0" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B608" s="0" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" s="0" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B609" s="0" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" s="0" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B610" s="0" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" s="0" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B611" s="0" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" s="0" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B612" s="0" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" s="0" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B613" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" s="0" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B614" s="0" t="s">
+        <v>1227</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
calibration analysis. not working very well, will try absolute time stamps
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="1584">
   <si>
     <t>GUID</t>
   </si>
@@ -3720,6 +3720,1074 @@
   </si>
   <si>
     <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jun-2023 22:38:57</t>
+  </si>
+  <si>
+    <t>000613</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:33:56</t>
+  </si>
+  <si>
+    <t>000614</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:39:47</t>
+  </si>
+  <si>
+    <t>000615</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:40:19</t>
+  </si>
+  <si>
+    <t>000616</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:41:27</t>
+  </si>
+  <si>
+    <t>000617</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:42:41</t>
+  </si>
+  <si>
+    <t>000618</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:42:58</t>
+  </si>
+  <si>
+    <t>000619</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:42:59</t>
+  </si>
+  <si>
+    <t>000620</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:43:06</t>
+  </si>
+  <si>
+    <t>000621</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:43:16</t>
+  </si>
+  <si>
+    <t>000622</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:43:25</t>
+  </si>
+  <si>
+    <t>000623</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:43:30</t>
+  </si>
+  <si>
+    <t>000624</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:43:38</t>
+  </si>
+  <si>
+    <t>000625</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:43:41</t>
+  </si>
+  <si>
+    <t>000626</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:43:45</t>
+  </si>
+  <si>
+    <t>000627</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:43:50</t>
+  </si>
+  <si>
+    <t>000628</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:43:53</t>
+  </si>
+  <si>
+    <t>000629</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:45:05</t>
+  </si>
+  <si>
+    <t>000630</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:48:48</t>
+  </si>
+  <si>
+    <t>000631</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:49:03</t>
+  </si>
+  <si>
+    <t>000632</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:49:34</t>
+  </si>
+  <si>
+    <t>000633</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:49:44</t>
+  </si>
+  <si>
+    <t>000634</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:50:18</t>
+  </si>
+  <si>
+    <t>000635</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:50:33</t>
+  </si>
+  <si>
+    <t>000636</t>
+  </si>
+  <si>
+    <t>Details: DEBUG Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:52:04</t>
+  </si>
+  <si>
+    <t>000637</t>
+  </si>
+  <si>
+    <t>Details: DEBUG Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:52:58</t>
+  </si>
+  <si>
+    <t>000638</t>
+  </si>
+  <si>
+    <t>Details: DEBUG Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:53:22</t>
+  </si>
+  <si>
+    <t>000639</t>
+  </si>
+  <si>
+    <t>Details: DEBUG Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:56:01</t>
+  </si>
+  <si>
+    <t>000640</t>
+  </si>
+  <si>
+    <t>Details: DEBUG Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 31B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:56:29</t>
+  </si>
+  <si>
+    <t>000641</t>
+  </si>
+  <si>
+    <t>Details: DEBUG Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 08:57:18</t>
+  </si>
+  <si>
+    <t>000642</t>
+  </si>
+  <si>
+    <t>Details: DEBUG Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:00:53</t>
+  </si>
+  <si>
+    <t>000643</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 11A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:17:06</t>
+  </si>
+  <si>
+    <t>000644</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 11B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:17:23</t>
+  </si>
+  <si>
+    <t>000645</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 00A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:21:44</t>
+  </si>
+  <si>
+    <t>000646</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 00B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:31:42</t>
+  </si>
+  <si>
+    <t>000647</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 11A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:32:12</t>
+  </si>
+  <si>
+    <t>000648</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 11B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:33:36</t>
+  </si>
+  <si>
+    <t>000649</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 11B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:38:00</t>
+  </si>
+  <si>
+    <t>000650</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 11B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:39:45</t>
+  </si>
+  <si>
+    <t>000651</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 11B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:42:03</t>
+  </si>
+  <si>
+    <t>000652</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 11B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:43:03</t>
+  </si>
+  <si>
+    <t>000653</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 12A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:45:25</t>
+  </si>
+  <si>
+    <t>000654</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 12A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:46:08</t>
+  </si>
+  <si>
+    <t>000655</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 12B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:47:38</t>
+  </si>
+  <si>
+    <t>000656</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 12B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:48:08</t>
+  </si>
+  <si>
+    <t>000657</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 13A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:49:09</t>
+  </si>
+  <si>
+    <t>000658</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 13A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 09:49:17</t>
+  </si>
+  <si>
+    <t>000659</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_PointToPoint.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibratrionAnalysis. Date Generated: 22-Jun-2023 10:19:14</t>
+  </si>
+  <si>
+    <t>000660</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_PointToPoint.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:19:31</t>
+  </si>
+  <si>
+    <t>000661</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:19:58</t>
+  </si>
+  <si>
+    <t>000662</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:20:17</t>
+  </si>
+  <si>
+    <t>000663</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:21:27</t>
+  </si>
+  <si>
+    <t>000664</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:21:45</t>
+  </si>
+  <si>
+    <t>000665</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:22:14</t>
+  </si>
+  <si>
+    <t>000666</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:22:35</t>
+  </si>
+  <si>
+    <t>000667</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:23:43</t>
+  </si>
+  <si>
+    <t>000668</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:23:59</t>
+  </si>
+  <si>
+    <t>000669</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:24:11</t>
+  </si>
+  <si>
+    <t>000670</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:24:18</t>
+  </si>
+  <si>
+    <t>000671</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:24:22</t>
+  </si>
+  <si>
+    <t>000672</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:24:28</t>
+  </si>
+  <si>
+    <t>000673</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:24:49</t>
+  </si>
+  <si>
+    <t>000674</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:26:35</t>
+  </si>
+  <si>
+    <t>000675</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:27:06</t>
+  </si>
+  <si>
+    <t>000676</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:27:46</t>
+  </si>
+  <si>
+    <t>000677</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:27:55</t>
+  </si>
+  <si>
+    <t>000678</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:28:08</t>
+  </si>
+  <si>
+    <t>000679</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:28:22</t>
+  </si>
+  <si>
+    <t>000680</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:28:31</t>
+  </si>
+  <si>
+    <t>000681</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:28:38</t>
+  </si>
+  <si>
+    <t>000682</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:28:46</t>
+  </si>
+  <si>
+    <t>000683</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:28:56</t>
+  </si>
+  <si>
+    <t>000684</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:28:59</t>
+  </si>
+  <si>
+    <t>000685</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:29:04</t>
+  </si>
+  <si>
+    <t>000686</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:29:09</t>
+  </si>
+  <si>
+    <t>000687</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:29:19</t>
+  </si>
+  <si>
+    <t>000688</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:30:36</t>
+  </si>
+  <si>
+    <t>000689</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:30:39</t>
+  </si>
+  <si>
+    <t>000690</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:30:44</t>
+  </si>
+  <si>
+    <t>000691</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:31:09</t>
+  </si>
+  <si>
+    <t>000692</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:31:22</t>
+  </si>
+  <si>
+    <t>000693</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:31:29</t>
+  </si>
+  <si>
+    <t>000694</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:31:38</t>
+  </si>
+  <si>
+    <t>000695</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:31:46</t>
+  </si>
+  <si>
+    <t>000696</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:33:04</t>
+  </si>
+  <si>
+    <t>000697</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:33:20</t>
+  </si>
+  <si>
+    <t>000698</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:33:28</t>
+  </si>
+  <si>
+    <t>000699</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:33:41</t>
+  </si>
+  <si>
+    <t>000700</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 13B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 10:34:26</t>
+  </si>
+  <si>
+    <t>000701</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 13B. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 10:35:33</t>
+  </si>
+  <si>
+    <t>000702</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 14A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 10:36:10</t>
+  </si>
+  <si>
+    <t>000703</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 14A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 10:36:49</t>
+  </si>
+  <si>
+    <t>000704</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 14A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 10:37:09</t>
+  </si>
+  <si>
+    <t>000705</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:37:42</t>
+  </si>
+  <si>
+    <t>000706</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:37:56</t>
+  </si>
+  <si>
+    <t>000707</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:38:32</t>
+  </si>
+  <si>
+    <t>000708</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:38:40</t>
+  </si>
+  <si>
+    <t>000709</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:38:45</t>
+  </si>
+  <si>
+    <t>000710</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:38:50</t>
+  </si>
+  <si>
+    <t>000711</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:38:55</t>
+  </si>
+  <si>
+    <t>000712</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 14C. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 10:40:38</t>
+  </si>
+  <si>
+    <t>000713</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 14C. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 10:44:01</t>
+  </si>
+  <si>
+    <t>000714</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14C_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14C. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:44:29</t>
+  </si>
+  <si>
+    <t>000715</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 14C. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 10:48:01</t>
+  </si>
+  <si>
+    <t>000716</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14C_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14C. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:52:17</t>
+  </si>
+  <si>
+    <t>000717</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14C_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14C. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:52:43</t>
+  </si>
+  <si>
+    <t>000718</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 10:53:04</t>
+  </si>
+  <si>
+    <t>000719</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp21A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_21A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:53:35</t>
+  </si>
+  <si>
+    <t>000720</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp21A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_21A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:54:14</t>
+  </si>
+  <si>
+    <t>000721</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:54:40</t>
+  </si>
+  <si>
+    <t>000722</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14C_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14C. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:54:50</t>
+  </si>
+  <si>
+    <t>000723</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14C_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14C. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:55:01</t>
+  </si>
+  <si>
+    <t>000724</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp14A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_14A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:55:08</t>
+  </si>
+  <si>
+    <t>000725</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:55:25</t>
+  </si>
+  <si>
+    <t>000726</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:56:16</t>
+  </si>
+  <si>
+    <t>000727</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:56:24</t>
+  </si>
+  <si>
+    <t>000728</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:56:30</t>
+  </si>
+  <si>
+    <t>000729</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:58:08</t>
+  </si>
+  <si>
+    <t>000730</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:58:52</t>
+  </si>
+  <si>
+    <t>000731</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:58:59</t>
+  </si>
+  <si>
+    <t>000732</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:59:13</t>
+  </si>
+  <si>
+    <t>000733</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:59:30</t>
+  </si>
+  <si>
+    <t>000734</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:59:37</t>
+  </si>
+  <si>
+    <t>000735</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:59:41</t>
+  </si>
+  <si>
+    <t>000736</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 10:59:45</t>
+  </si>
+  <si>
+    <t>000737</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00B - Euclidean distance underneath.. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:00:40</t>
+  </si>
+  <si>
+    <t>000738</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:01:10</t>
+  </si>
+  <si>
+    <t>000739</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:01:23</t>
+  </si>
+  <si>
+    <t>000740</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:01:43</t>
+  </si>
+  <si>
+    <t>000741</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:01:52</t>
+  </si>
+  <si>
+    <t>000742</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:01:56</t>
+  </si>
+  <si>
+    <t>000743</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:02:01</t>
+  </si>
+  <si>
+    <t>000744</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:02:05</t>
+  </si>
+  <si>
+    <t>000745</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:02:09</t>
+  </si>
+  <si>
+    <t>000746</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 00B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp00B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_00B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:02:14</t>
+  </si>
+  <si>
+    <t>000747</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:02:55</t>
+  </si>
+  <si>
+    <t>000748</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:03:01</t>
+  </si>
+  <si>
+    <t>000749</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:03:07</t>
+  </si>
+  <si>
+    <t>000750</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:03:08</t>
+  </si>
+  <si>
+    <t>000751</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:03:12</t>
+  </si>
+  <si>
+    <t>000752</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:03:19</t>
+  </si>
+  <si>
+    <t>000753</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 12A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:04:44</t>
+  </si>
+  <si>
+    <t>000754</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 12B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:05:07</t>
+  </si>
+  <si>
+    <t>000755</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 12B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:05:13</t>
+  </si>
+  <si>
+    <t>000756</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 12B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:05:38</t>
+  </si>
+  <si>
+    <t>000757</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 12B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:05:43</t>
+  </si>
+  <si>
+    <t>000758</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:06:39</t>
+  </si>
+  <si>
+    <t>000759</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:06:44</t>
+  </si>
+  <si>
+    <t>000760</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:06:48</t>
+  </si>
+  <si>
+    <t>000761</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:06:51</t>
+  </si>
+  <si>
+    <t>000762</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:07:09</t>
+  </si>
+  <si>
+    <t>000763</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:07:15</t>
+  </si>
+  <si>
+    <t>000764</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:07:20</t>
+  </si>
+  <si>
+    <t>000765</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:07:27</t>
+  </si>
+  <si>
+    <t>000766</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:07:34</t>
+  </si>
+  <si>
+    <t>000767</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 22-Jun-2023 11:07:39</t>
+  </si>
+  <si>
+    <t>000768</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:10:52</t>
+  </si>
+  <si>
+    <t>000769</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:11:26</t>
+  </si>
+  <si>
+    <t>000770</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:15:53</t>
+  </si>
+  <si>
+    <t>000771</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:17:05</t>
+  </si>
+  <si>
+    <t>000772</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:17:24</t>
+  </si>
+  <si>
+    <t>000773</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:17:36</t>
+  </si>
+  <si>
+    <t>000774</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:23:55</t>
+  </si>
+  <si>
+    <t>000775</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:24:23</t>
+  </si>
+  <si>
+    <t>000776</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:25:37</t>
+  </si>
+  <si>
+    <t>000777</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:26:11</t>
+  </si>
+  <si>
+    <t>000778</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:26:22</t>
+  </si>
+  <si>
+    <t>000779</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:30:09</t>
+  </si>
+  <si>
+    <t>000780</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:30:19</t>
+  </si>
+  <si>
+    <t>000781</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:30:34</t>
+  </si>
+  <si>
+    <t>000782</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:30:44</t>
+  </si>
+  <si>
+    <t>000783</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 21A. Experiment ID: 21A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:33:04</t>
+  </si>
+  <si>
+    <t>000784</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 13A. Experiment ID: 13A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:34:13</t>
+  </si>
+  <si>
+    <t>000785</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 13A. Experiment ID: 13A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:34:29</t>
+  </si>
+  <si>
+    <t>000786</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 13A. Experiment ID: 13A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:34:43</t>
+  </si>
+  <si>
+    <t>000787</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 41A. Experiment ID: 41A. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:37:36</t>
+  </si>
+  <si>
+    <t>000788</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 41C. Experiment ID: 41C. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:38:15</t>
+  </si>
+  <si>
+    <t>000789</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 41C. Experiment ID: 41C. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:38:33</t>
+  </si>
+  <si>
+    <t>000790</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 41C. Experiment ID: 41C. Script used: Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 22-Jun-2023 11:39:09</t>
   </si>
 </sst>
 </file>
@@ -4089,7 +5157,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B614"/>
+  <dimension ref="A1:B792"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -9013,6 +10081,1430 @@
         <v>1227</v>
       </c>
     </row>
+    <row r="615">
+      <c r="A615" s="0" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B615" s="0" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" s="0" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B616" s="0" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" s="0" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B617" s="0" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" s="0" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B618" s="0" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" s="0" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B619" s="0" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" s="0" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B620" s="0" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" s="0" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B621" s="0" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" s="0" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B622" s="0" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" s="0" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B623" s="0" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" s="0" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B624" s="0" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" s="0" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B625" s="0" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" s="0" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B626" s="0" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" s="0" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B627" s="0" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" s="0" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B628" s="0" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" s="0" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B629" s="0" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" s="0" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B630" s="0" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" s="0" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B631" s="0" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" s="0" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B632" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" s="0" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B633" s="0" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" s="0" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B634" s="0" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" s="0" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B635" s="0" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B636" s="0" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" s="0" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B637" s="0" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" s="0" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B638" s="0" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B639" s="0" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B640" s="0" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" s="0" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B641" s="0" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" s="0" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B642" s="0" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" s="0" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B643" s="0" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" s="0" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B644" s="0" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" s="0" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B645" s="0" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" s="0" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B646" s="0" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B647" s="0" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B648" s="0" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B649" s="0" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" s="0" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B650" s="0" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" s="0" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B651" s="0" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" s="0" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B652" s="0" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B653" s="0" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" s="0" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B654" s="0" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" s="0" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B655" s="0" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" s="0" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B656" s="0" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" s="0" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B657" s="0" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B658" s="0" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" s="0" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B659" s="0" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" s="0" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B660" s="0" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" s="0" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B661" s="0" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" s="0" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B662" s="0" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" s="0" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B663" s="0" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" s="0" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B664" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" s="0" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B665" s="0" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" s="0" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B666" s="0" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" s="0" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B667" s="0" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" s="0" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B668" s="0" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" s="0" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B669" s="0" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" s="0" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B670" s="0" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" s="0" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B671" s="0" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" s="0" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B672" s="0" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" s="0" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B673" s="0" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" s="0" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B674" s="0" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" s="0" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B675" s="0" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" s="0" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B676" s="0" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" s="0" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B677" s="0" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" s="0" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B678" s="0" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" s="0" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B679" s="0" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" s="0" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B680" s="0" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" s="0" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B681" s="0" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" s="0" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B682" s="0" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" s="0" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B683" s="0" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" s="0" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B684" s="0" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" s="0" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B685" s="0" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" s="0" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B686" s="0" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" s="0" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B687" s="0" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" s="0" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B688" s="0" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" s="0" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B689" s="0" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" s="0" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B690" s="0" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" s="0" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B691" s="0" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" s="0" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B692" s="0" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" s="0" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B693" s="0" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" s="0" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B694" s="0" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" s="0" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B695" s="0" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" s="0" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B696" s="0" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" s="0" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B697" s="0" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" s="0" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B698" s="0" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" s="0" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B699" s="0" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" s="0" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B700" s="0" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" s="0" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B701" s="0" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" s="0" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B702" s="0" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" s="0" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B703" s="0" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" s="0" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B704" s="0" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" s="0" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B705" s="0" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" s="0" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B706" s="0" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" s="0" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B707" s="0" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" s="0" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B708" s="0" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" s="0" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B709" s="0" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" s="0" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B710" s="0" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" s="0" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B711" s="0" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" s="0" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B712" s="0" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" s="0" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B713" s="0" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" s="0" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B714" s="0" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" s="0" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B715" s="0" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" s="0" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B716" s="0" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" s="0" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B717" s="0" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" s="0" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B718" s="0" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" s="0" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B719" s="0" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" s="0" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B720" s="0" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" s="0" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B721" s="0" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" s="0" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B722" s="0" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" s="0" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B723" s="0" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" s="0" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B724" s="0" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" s="0" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B725" s="0" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" s="0" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B726" s="0" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" s="0" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B727" s="0" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" s="0" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B728" s="0" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" s="0" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B729" s="0" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" s="0" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B730" s="0" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" s="0" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B731" s="0" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" s="0" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B732" s="0" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" s="0" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B733" s="0" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" s="0" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B734" s="0" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" s="0" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B735" s="0" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" s="0" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B736" s="0" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" s="0" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B737" s="0" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" s="0" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B738" s="0" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" s="0" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B739" s="0" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" s="0" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B740" s="0" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" s="0" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B741" s="0" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" s="0" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B742" s="0" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" s="0" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B743" s="0" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" s="0" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B744" s="0" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" s="0" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B745" s="0" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" s="0" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B746" s="0" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" s="0" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B747" s="0" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" s="0" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B748" s="0" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" s="0" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B749" s="0" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" s="0" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B750" s="0" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" s="0" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B751" s="0" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" s="0" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B752" s="0" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" s="0" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B753" s="0" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" s="0" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B754" s="0" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" s="0" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B755" s="0" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" s="0" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B756" s="0" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" s="0" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B757" s="0" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" s="0" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B758" s="0" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" s="0" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B759" s="0" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" s="0" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B760" s="0" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" s="0" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B761" s="0" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" s="0" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B762" s="0" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" s="0" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B763" s="0" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B764" s="0" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" s="0" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B765" s="0" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" s="0" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B766" s="0" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" s="0" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B767" s="0" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" s="0" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B768" s="0" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" s="0" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B769" s="0" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" s="0" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B770" s="0" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" s="0" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B771" s="0" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" s="0" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B772" s="0" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" s="0" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B773" s="0" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" s="0" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B774" s="0" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" s="0" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B775" s="0" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" s="0" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B776" s="0" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" s="0" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B777" s="0" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" s="0" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B778" s="0" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" s="0" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B779" s="0" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" s="0" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B780" s="0" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" s="0" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B781" s="0" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" s="0" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B782" s="0" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" s="0" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B783" s="0" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" s="0" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B784" s="0" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" s="0" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B785" s="0" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" s="0" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B786" s="0" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" s="0" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B787" s="0" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" s="0" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B788" s="0" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" s="0" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B789" s="0" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" s="0" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B790" s="0" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" s="0" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B791" s="0" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" s="0" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B792" s="0" t="s">
+        <v>1583</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
extraneous movement averages visualised with individual cycles behind in grey.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="1606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="1662">
   <si>
     <t>GUID</t>
   </si>
@@ -4854,6 +4854,174 @@
   </si>
   <si>
     <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_B1_001_SavedCycle_3_Resampled. Script used: ResampledVisualisationCycleAverage_XY.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\SavedCycles_Resampled\Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_B1_Resampled_Average_Figures. Date Generated: 29-Jun-2023 15:44:03</t>
+  </si>
+  <si>
+    <t>000802</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 29-Jun-2023 16:01:49</t>
+  </si>
+  <si>
+    <t>000803</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:03:24</t>
+  </si>
+  <si>
+    <t>000804</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:03:58</t>
+  </si>
+  <si>
+    <t>000805</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:05:55</t>
+  </si>
+  <si>
+    <t>000806</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:06:14</t>
+  </si>
+  <si>
+    <t>000807</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:06:56</t>
+  </si>
+  <si>
+    <t>000808</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Knees. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:07:13</t>
+  </si>
+  <si>
+    <t>000809</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Waist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_C1_001_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:07:54</t>
+  </si>
+  <si>
+    <t>000810</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Waist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_C1_001_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:10:20</t>
+  </si>
+  <si>
+    <t>000811</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:11:07</t>
+  </si>
+  <si>
+    <t>000812</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:11:10</t>
+  </si>
+  <si>
+    <t>000813</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:11:41</t>
+  </si>
+  <si>
+    <t>000814</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:11:47</t>
+  </si>
+  <si>
+    <t>000815</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:12:26</t>
+  </si>
+  <si>
+    <t>000816</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:12:33</t>
+  </si>
+  <si>
+    <t>000817</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:12:41</t>
+  </si>
+  <si>
+    <t>000818</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:12:46</t>
+  </si>
+  <si>
+    <t>000819</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:13:09</t>
+  </si>
+  <si>
+    <t>000820</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:13:25</t>
+  </si>
+  <si>
+    <t>000821</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Waist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_C1_001_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:13:44</t>
+  </si>
+  <si>
+    <t>000822</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Knees. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:14:02</t>
+  </si>
+  <si>
+    <t>000823</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Wrist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_E1_001_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:14:29</t>
+  </si>
+  <si>
+    <t>000824</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Wrist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_E1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:14:50</t>
+  </si>
+  <si>
+    <t>000825</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Wrist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_E1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:16:10</t>
+  </si>
+  <si>
+    <t>000826</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:17:06</t>
+  </si>
+  <si>
+    <t>000827</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:17:14</t>
+  </si>
+  <si>
+    <t>000828</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:18:14</t>
+  </si>
+  <si>
+    <t>000829</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:18:28</t>
   </si>
 </sst>
 </file>
@@ -5223,7 +5391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B803"/>
+  <dimension ref="A1:B831"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -5231,8 +5399,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="557.42578125" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="7.16796875" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="524.89453125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
@@ -11657,6 +11825,230 @@
       </c>
       <c r="B803" s="0" t="s">
         <v>1605</v>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" s="0" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B804" s="0" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" s="0" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B805" s="0" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" s="0" t="s">
+        <v>1610</v>
+      </c>
+      <c r="B806" s="0" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" s="0" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B807" s="0" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" s="0" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B808" s="0" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" s="0" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B809" s="0" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" s="0" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B810" s="0" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" s="0" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B811" s="0" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" s="0" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B812" s="0" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" s="0" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B813" s="0" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" s="0" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B814" s="0" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" s="0" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B815" s="0" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" s="0" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B816" s="0" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" s="0" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B817" s="0" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" s="0" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B818" s="0" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" s="0" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B819" s="0" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" s="0" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B820" s="0" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" s="0" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B821" s="0" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" s="0" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B822" s="0" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" s="0" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B823" s="0" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" s="0" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B824" s="0" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" s="0" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B825" s="0" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" s="0" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B826" s="0" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" s="0" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B827" s="0" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" s="0" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B828" s="0" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" s="0" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B829" s="0" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" s="0" t="s">
+        <v>1658</v>
+      </c>
+      <c r="B830" s="0" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" s="0" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B831" s="0" t="s">
+        <v>1661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better quality figures for averages of extraneous movements
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="1662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="1860">
   <si>
     <t>GUID</t>
   </si>
@@ -5022,6 +5022,600 @@
   </si>
   <si>
     <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:18:28</t>
+  </si>
+  <si>
+    <t>000830</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:28:11</t>
+  </si>
+  <si>
+    <t>000831</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:28:36</t>
+  </si>
+  <si>
+    <t>000832</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:29:18</t>
+  </si>
+  <si>
+    <t>000833</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:31:21</t>
+  </si>
+  <si>
+    <t>000834</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:31:51</t>
+  </si>
+  <si>
+    <t>000835</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:31:56</t>
+  </si>
+  <si>
+    <t>000836</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:32:50</t>
+  </si>
+  <si>
+    <t>000837</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:58:33</t>
+  </si>
+  <si>
+    <t>000838</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:58:38</t>
+  </si>
+  <si>
+    <t>000839</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 16:59:27</t>
+  </si>
+  <si>
+    <t>000840</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:01:46</t>
+  </si>
+  <si>
+    <t>000841</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:01:57</t>
+  </si>
+  <si>
+    <t>000842</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:02:06</t>
+  </si>
+  <si>
+    <t>000843</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:02:55</t>
+  </si>
+  <si>
+    <t>000844</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:04:41</t>
+  </si>
+  <si>
+    <t>000845</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:05:20</t>
+  </si>
+  <si>
+    <t>000846</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:05:25</t>
+  </si>
+  <si>
+    <t>000847</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:05:34</t>
+  </si>
+  <si>
+    <t>000848</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:05:42</t>
+  </si>
+  <si>
+    <t>000849</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:05:48</t>
+  </si>
+  <si>
+    <t>000850</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:06:37</t>
+  </si>
+  <si>
+    <t>000851</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:06:50</t>
+  </si>
+  <si>
+    <t>000852</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:06:59</t>
+  </si>
+  <si>
+    <t>000853</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:07:09</t>
+  </si>
+  <si>
+    <t>000854</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:07:54</t>
+  </si>
+  <si>
+    <t>000855</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:08:01</t>
+  </si>
+  <si>
+    <t>000856</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:08:13</t>
+  </si>
+  <si>
+    <t>000857</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:08:19</t>
+  </si>
+  <si>
+    <t>000858</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:08:44</t>
+  </si>
+  <si>
+    <t>000859</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:08:50</t>
+  </si>
+  <si>
+    <t>000860</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:09:17</t>
+  </si>
+  <si>
+    <t>000861</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:10:48</t>
+  </si>
+  <si>
+    <t>000862</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:10:53</t>
+  </si>
+  <si>
+    <t>000863</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:11:28</t>
+  </si>
+  <si>
+    <t>000864</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:11:41</t>
+  </si>
+  <si>
+    <t>000865</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:11:55</t>
+  </si>
+  <si>
+    <t>000866</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:12:09</t>
+  </si>
+  <si>
+    <t>000867</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:12:15</t>
+  </si>
+  <si>
+    <t>000868</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:13:24</t>
+  </si>
+  <si>
+    <t>000869</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:13:29</t>
+  </si>
+  <si>
+    <t>000870</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:13:37</t>
+  </si>
+  <si>
+    <t>000871</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:13:42</t>
+  </si>
+  <si>
+    <t>000872</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:14:17</t>
+  </si>
+  <si>
+    <t>000873</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:14:34</t>
+  </si>
+  <si>
+    <t>000874</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:15:16</t>
+  </si>
+  <si>
+    <t>000875</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:15:34</t>
+  </si>
+  <si>
+    <t>000876</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:16:35</t>
+  </si>
+  <si>
+    <t>000877</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:17:22</t>
+  </si>
+  <si>
+    <t>000878</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:20:12</t>
+  </si>
+  <si>
+    <t>000879</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:20:28</t>
+  </si>
+  <si>
+    <t>000880</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:20:39</t>
+  </si>
+  <si>
+    <t>000881</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:20:46</t>
+  </si>
+  <si>
+    <t>000882</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:21:03</t>
+  </si>
+  <si>
+    <t>000883</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:21:08</t>
+  </si>
+  <si>
+    <t>000884</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:21:53</t>
+  </si>
+  <si>
+    <t>000885</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:22:00</t>
+  </si>
+  <si>
+    <t>000886</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:22:18</t>
+  </si>
+  <si>
+    <t>000887</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:23:10</t>
+  </si>
+  <si>
+    <t>000888</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:23:16</t>
+  </si>
+  <si>
+    <t>000889</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:23:28</t>
+  </si>
+  <si>
+    <t>000890</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:24:36</t>
+  </si>
+  <si>
+    <t>000891</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:24:41</t>
+  </si>
+  <si>
+    <t>000892</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:25:20</t>
+  </si>
+  <si>
+    <t>000893</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:25:23</t>
+  </si>
+  <si>
+    <t>000894</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:25:30</t>
+  </si>
+  <si>
+    <t>000895</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:25:33</t>
+  </si>
+  <si>
+    <t>000896</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:25:36</t>
+  </si>
+  <si>
+    <t>000897</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:26:40</t>
+  </si>
+  <si>
+    <t>000898</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:27:36</t>
+  </si>
+  <si>
+    <t>000899</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:27:46</t>
+  </si>
+  <si>
+    <t>000900</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:28:04</t>
+  </si>
+  <si>
+    <t>000901</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: LiveEditorEvaluationHelperE1480619866.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:28:08</t>
+  </si>
+  <si>
+    <t>000902</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:28:50</t>
+  </si>
+  <si>
+    <t>000903</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:28:56</t>
+  </si>
+  <si>
+    <t>000904</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:29:04</t>
+  </si>
+  <si>
+    <t>000905</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:31:30</t>
+  </si>
+  <si>
+    <t>000906</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:31:42</t>
+  </si>
+  <si>
+    <t>000907</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:32:04</t>
+  </si>
+  <si>
+    <t>000908</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:32:20</t>
+  </si>
+  <si>
+    <t>000909</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:32:35</t>
+  </si>
+  <si>
+    <t>000910</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:33:47</t>
+  </si>
+  <si>
+    <t>000911</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:34:01</t>
+  </si>
+  <si>
+    <t>000912</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:34:09</t>
+  </si>
+  <si>
+    <t>000913</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:34:45</t>
+  </si>
+  <si>
+    <t>000914</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:35:17</t>
+  </si>
+  <si>
+    <t>000915</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:35:47</t>
+  </si>
+  <si>
+    <t>000916</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Upper_Arm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:35:59</t>
+  </si>
+  <si>
+    <t>000917</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:36:33</t>
+  </si>
+  <si>
+    <t>000918</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Waist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_C1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:36:55</t>
+  </si>
+  <si>
+    <t>000919</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Knees. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:37:23</t>
+  </si>
+  <si>
+    <t>000920</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Knees. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_B1_001_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:38:24</t>
+  </si>
+  <si>
+    <t>000921</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Waist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_C1_001_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:38:51</t>
+  </si>
+  <si>
+    <t>000922</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Waist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_C1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:39:29</t>
+  </si>
+  <si>
+    <t>000923</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Feet. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_D1_002_SavedCycle_3_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:40:24</t>
+  </si>
+  <si>
+    <t>000924</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Wrist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_E1_001_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:41:09</t>
+  </si>
+  <si>
+    <t>000925</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Wrist. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_E1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:41:21</t>
+  </si>
+  <si>
+    <t>000926</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_UpperArm. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_F1_001_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:41:43</t>
+  </si>
+  <si>
+    <t>000927</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Control. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_A1_006_SavedCycle_5_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:42:17</t>
+  </si>
+  <si>
+    <t>000928</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Control. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_A1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:42:38</t>
   </si>
 </sst>
 </file>
@@ -5391,7 +5985,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B831"/>
+  <dimension ref="A1:B930"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -5399,8 +5993,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.16796875" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="524.89453125" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="7.140625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="557.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
@@ -12049,6 +12643,798 @@
       </c>
       <c r="B831" s="0" t="s">
         <v>1661</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" s="0" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B832" s="0" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" s="0" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B833" s="0" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" s="0" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B834" s="0" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" s="0" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B835" s="0" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" s="0" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B836" s="0" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" s="0" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B837" s="0" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" s="0" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B838" s="0" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" s="0" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B839" s="0" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" s="0" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B840" s="0" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" s="0" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B841" s="0" t="s">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" s="0" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B842" s="0" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" s="0" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B843" s="0" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" s="0" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B844" s="0" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" s="0" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B845" s="0" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" s="0" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B846" s="0" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" s="0" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B847" s="0" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" s="0" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B848" s="0" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" s="0" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B849" s="0" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" s="0" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B850" s="0" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" s="0" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B851" s="0" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" s="0" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B852" s="0" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" s="0" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B853" s="0" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" s="0" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B854" s="0" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" s="0" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B855" s="0" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" s="0" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B856" s="0" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" s="0" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B857" s="0" t="s">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" s="0" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B858" s="0" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" s="0" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B859" s="0" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" s="0" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B860" s="0" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" s="0" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B861" s="0" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" s="0" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B862" s="0" t="s">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" s="0" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B863" s="0" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" s="0" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B864" s="0" t="s">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" s="0" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B865" s="0" t="s">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" s="0" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B866" s="0" t="s">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" s="0" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B867" s="0" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" s="0" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B868" s="0" t="s">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" s="0" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B869" s="0" t="s">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" s="0" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B870" s="0" t="s">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" s="0" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B871" s="0" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" s="0" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B872" s="0" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" s="0" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B873" s="0" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" s="0" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B874" s="0" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" s="0" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B875" s="0" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" s="0" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B876" s="0" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" s="0" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B877" s="0" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" s="0" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B878" s="0" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" s="0" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B879" s="0" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" s="0" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B880" s="0" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" s="0" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B881" s="0" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" s="0" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B882" s="0" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" s="0" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B883" s="0" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" s="0" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B884" s="0" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" s="0" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B885" s="0" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" s="0" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B886" s="0" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" s="0" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B887" s="0" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" s="0" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B888" s="0" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" s="0" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B889" s="0" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" s="0" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B890" s="0" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" s="0" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B891" s="0" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" s="0" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B892" s="0" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" s="0" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B893" s="0" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" s="0" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B894" s="0" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" s="0" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B895" s="0" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" s="0" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B896" s="0" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" s="0" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B897" s="0" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" s="0" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B898" s="0" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" s="0" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B899" s="0" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" s="0" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B900" s="0" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" s="0" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B901" s="0" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" s="0" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B902" s="0" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" s="0" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B903" s="0" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" s="0" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B904" s="0" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" s="0" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B905" s="0" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" s="0" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B906" s="0" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" s="0" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B907" s="0" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" s="0" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B908" s="0" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" s="0" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B909" s="0" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" s="0" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B910" s="0" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" s="0" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B911" s="0" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" s="0" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B912" s="0" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" s="0" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B913" s="0" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="0" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B914" s="0" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" s="0" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B915" s="0" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" s="0" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B916" s="0" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" s="0" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B917" s="0" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" s="0" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B918" s="0" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" s="0" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B919" s="0" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" s="0" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B920" s="0" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" s="0" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B921" s="0" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" s="0" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B922" s="0" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" s="0" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B923" s="0" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" s="0" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B924" s="0" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" s="0" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B925" s="0" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" s="0" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B926" s="0" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" s="0" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B927" s="0" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" s="0" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B928" s="0" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" s="0" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B929" s="0" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" s="0" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B930" s="0" t="s">
+        <v>1859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
raw collection now uses epochs. system calculation of baton tip works properly. can be split by time.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="1860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="2042">
   <si>
     <t>GUID</t>
   </si>
@@ -5616,6 +5616,552 @@
   </si>
   <si>
     <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Control. Script used: ResampledVisualisationCycles_XY.  Dataset used: Session01_Exp_A1_006_SavedCycle_4_Resampled.mat. File Location: Visualisations/Session01_Resampled_Average_Figures. Date Generated: 29-Jun-2023 17:42:38</t>
+  </si>
+  <si>
+    <t>000929</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 11B. Experiment ID: 11B. Script used: Step3_Interpret_IMU_And_LeapDevice_And_Motive_Separately.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 02-Jul-2023 14:19:12</t>
+  </si>
+  <si>
+    <t>000930</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:22:37</t>
+  </si>
+  <si>
+    <t>000931</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:25:55</t>
+  </si>
+  <si>
+    <t>000932</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:28:57</t>
+  </si>
+  <si>
+    <t>000933</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:29:40</t>
+  </si>
+  <si>
+    <t>000934</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:29:57</t>
+  </si>
+  <si>
+    <t>000935</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:30:12</t>
+  </si>
+  <si>
+    <t>000936</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 1 and last 0 points of IMU, 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:31:12</t>
+  </si>
+  <si>
+    <t>000937</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 1 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:31:23</t>
+  </si>
+  <si>
+    <t>000938</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 50 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:37:02</t>
+  </si>
+  <si>
+    <t>000939</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 25 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:37:20</t>
+  </si>
+  <si>
+    <t>000940</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 40 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:37:27</t>
+  </si>
+  <si>
+    <t>000941</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 50 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:37:32</t>
+  </si>
+  <si>
+    <t>000942</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:37:37</t>
+  </si>
+  <si>
+    <t>000943</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:37:38</t>
+  </si>
+  <si>
+    <t>000944</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 40 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:37:44</t>
+  </si>
+  <si>
+    <t>000945</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:37:48</t>
+  </si>
+  <si>
+    <t>000946</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:37:48</t>
+  </si>
+  <si>
+    <t>000947</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 10 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:38:23</t>
+  </si>
+  <si>
+    <t>000948</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 10 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:38:24</t>
+  </si>
+  <si>
+    <t>000949</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 2 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:38:54</t>
+  </si>
+  <si>
+    <t>000950</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 5 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:38:58</t>
+  </si>
+  <si>
+    <t>000951</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:39:03</t>
+  </si>
+  <si>
+    <t>000952</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 3 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:39:07</t>
+  </si>
+  <si>
+    <t>000953</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:39:11</t>
+  </si>
+  <si>
+    <t>000954</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:45:09</t>
+  </si>
+  <si>
+    <t>000955</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:46:01</t>
+  </si>
+  <si>
+    <t>000956</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 50 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:47:23</t>
+  </si>
+  <si>
+    <t>000957</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 50 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:47:54</t>
+  </si>
+  <si>
+    <t>000958</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 50 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:48:01</t>
+  </si>
+  <si>
+    <t>000959</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 50 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:48:06</t>
+  </si>
+  <si>
+    <t>000960</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 50 and last 0 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:48:07</t>
+  </si>
+  <si>
+    <t>000961</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 4 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:48:33</t>
+  </si>
+  <si>
+    <t>000962</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 20 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:48:53</t>
+  </si>
+  <si>
+    <t>000963</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 50 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:49:02</t>
+  </si>
+  <si>
+    <t>000964</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 80 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:49:25</t>
+  </si>
+  <si>
+    <t>000965</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 110 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:49:33</t>
+  </si>
+  <si>
+    <t>000966</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 55 and last 110 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:50:52</t>
+  </si>
+  <si>
+    <t>000967</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 42 and last 110 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:51:04</t>
+  </si>
+  <si>
+    <t>000968</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 110 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:51:10</t>
+  </si>
+  <si>
+    <t>000969</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 140 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:51:32</t>
+  </si>
+  <si>
+    <t>000970</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 160 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:51:48</t>
+  </si>
+  <si>
+    <t>000971</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 160 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:52:27</t>
+  </si>
+  <si>
+    <t>000972</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 140 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:52:55</t>
+  </si>
+  <si>
+    <t>000973</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 150 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:53:02</t>
+  </si>
+  <si>
+    <t>000974</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 150 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:55:25</t>
+  </si>
+  <si>
+    <t>000975</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 150 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:56:00</t>
+  </si>
+  <si>
+    <t>000976</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 02-Jul-2023 14:56:39</t>
+  </si>
+  <si>
+    <t>000977</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 02-Jul-2023 14:56:49</t>
+  </si>
+  <si>
+    <t>000978</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 02-Jul-2023 14:57:20</t>
+  </si>
+  <si>
+    <t>000979</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 45 and last 150 points of IMU - 1st 50 and last 20 points of Motive) - Session02_SmoothBatonPosition - 13A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp13A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_13A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:58:02</t>
+  </si>
+  <si>
+    <t>000980</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 1 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:59:31</t>
+  </si>
+  <si>
+    <t>000981</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 50 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 14:59:50</t>
+  </si>
+  <si>
+    <t>000982</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 20 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:00</t>
+  </si>
+  <si>
+    <t>000983</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 30 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:07</t>
+  </si>
+  <si>
+    <t>000984</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 40 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:11</t>
+  </si>
+  <si>
+    <t>000985</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 50 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:16</t>
+  </si>
+  <si>
+    <t>000986</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 1 and last 20 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:23</t>
+  </si>
+  <si>
+    <t>000987</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 10 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:28</t>
+  </si>
+  <si>
+    <t>000988</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 20 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:33</t>
+  </si>
+  <si>
+    <t>000989</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 15 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:37</t>
+  </si>
+  <si>
+    <t>000990</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 12 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:43</t>
+  </si>
+  <si>
+    <t>000991</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 0 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:00:48</t>
+  </si>
+  <si>
+    <t>000992</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:01:28</t>
+  </si>
+  <si>
+    <t>000993</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 30 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:01:33</t>
+  </si>
+  <si>
+    <t>000994</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 1 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:01:38</t>
+  </si>
+  <si>
+    <t>000995</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 20 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:02:15</t>
+  </si>
+  <si>
+    <t>000996</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 50 and last 0 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:02:27</t>
+  </si>
+  <si>
+    <t>000997</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 50 and last 100 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:02:36</t>
+  </si>
+  <si>
+    <t>000998</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 50 and last 100 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:02:56</t>
+  </si>
+  <si>
+    <t>000999</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 50 and last 100 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:04:18</t>
+  </si>
+  <si>
+    <t>001000</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 50 and last 300 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:04:32</t>
+  </si>
+  <si>
+    <t>001001</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 50 and last 200 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:04:41</t>
+  </si>
+  <si>
+    <t>001002</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 50 and last 100 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:04:51</t>
+  </si>
+  <si>
+    <t>001003</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 14 and last 50 points of IMU - 1st 50 and last 150 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:04:59</t>
+  </si>
+  <si>
+    <t>001004</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration PCR (without 1st 20 and last 50 points of IMU - 1st 50 and last 150 points of Motive) - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 02-Jul-2023 15:05:46</t>
+  </si>
+  <si>
+    <t>001005</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Interpret_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 05-Jul-2023 19:33:56</t>
+  </si>
+  <si>
+    <t>001006</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 11B. Experiment ID: 11B. Script used: Step5_Interpret_Separately_TimeSynced.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 05-Jul-2023 19:58:38</t>
+  </si>
+  <si>
+    <t>001007</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 42E. Experiment ID: 42E. Script used: Step5_Interpret_Separately_TimeSynced.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 05-Jul-2023 20:04:33</t>
+  </si>
+  <si>
+    <t>001008</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 42E. Experiment ID: 42E. Script used: Step5_Interpret_Separately_TimeSynced.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 05-Jul-2023 20:06:22</t>
+  </si>
+  <si>
+    <t>001009</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 42E. Experiment ID: 42E. Script used: Step5_Interpret_Separately_TimeSynced.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 05-Jul-2023 20:06:45</t>
+  </si>
+  <si>
+    <t>001010</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading and Motive (OptiTrack) Reading experiment 42E. Experiment ID: 42E. Script used: Step5_Interpret_Separately_TimeSynced.  Dataset used: Test data from raw imu reading and raw leap reading with motive Data scaled and resampled. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 05-Jul-2023 20:06:49</t>
+  </si>
+  <si>
+    <t>001011</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:10:52</t>
+  </si>
+  <si>
+    <t>001012</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:12:04</t>
+  </si>
+  <si>
+    <t>001013</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:14:34</t>
+  </si>
+  <si>
+    <t>001014</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:15:34</t>
+  </si>
+  <si>
+    <t>001015</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:15:42</t>
+  </si>
+  <si>
+    <t>001016</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:16:38</t>
+  </si>
+  <si>
+    <t>001017</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_003_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_003_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:16:41</t>
+  </si>
+  <si>
+    <t>001018</t>
+  </si>
+  <si>
+    <t>Details: 60bpm_mf_44path_Normal_SplitCycles_TimeBased_Session01_Exp_A1_002_tXYZ.mat. Script used: IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session01_ManipulatedData\Session01_Exp_A1_002_tXYZ.mat. File Location: Visualisations/Session01_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:17:06</t>
+  </si>
+  <si>
+    <t>001019</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:18:52</t>
   </si>
 </sst>
 </file>
@@ -5985,7 +6531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B930"/>
+  <dimension ref="A1:B1021"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -13437,6 +13983,734 @@
         <v>1859</v>
       </c>
     </row>
+    <row r="931">
+      <c r="A931" s="0" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B931" s="0" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" s="0" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B932" s="0" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" s="0" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B933" s="0" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" s="0" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B934" s="0" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" s="0" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B935" s="0" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" s="0" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B936" s="0" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" s="0" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B937" s="0" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" s="0" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B938" s="0" t="s">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" s="0" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B939" s="0" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" s="0" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B940" s="0" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" s="0" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B941" s="0" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" s="0" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B942" s="0" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" s="0" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B943" s="0" t="s">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" s="0" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B944" s="0" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" s="0" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B945" s="0" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" s="0" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B946" s="0" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" s="0" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B947" s="0" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" s="0" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B948" s="0" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" s="0" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B949" s="0" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" s="0" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B950" s="0" t="s">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" s="0" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B951" s="0" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" s="0" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B952" s="0" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" s="0" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B953" s="0" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" s="0" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B954" s="0" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" s="0" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B955" s="0" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" s="0" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B956" s="0" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" s="0" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B957" s="0" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" s="0" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B958" s="0" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" s="0" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B959" s="0" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" s="0" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B960" s="0" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" s="0" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B961" s="0" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" s="0" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B962" s="0" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" s="0" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B963" s="0" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" s="0" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B964" s="0" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" s="0" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B965" s="0" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" s="0" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B966" s="0" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" s="0" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B967" s="0" t="s">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" s="0" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B968" s="0" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" s="0" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B969" s="0" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" s="0" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B970" s="0" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" s="0" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B971" s="0" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" s="0" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B972" s="0" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" s="0" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B973" s="0" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" s="0" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B974" s="0" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" s="0" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B975" s="0" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" s="0" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B976" s="0" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" s="0" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B977" s="0" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" s="0" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B978" s="0" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" s="0" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B979" s="0" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" s="0" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B980" s="0" t="s">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" s="0" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B981" s="0" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" s="0" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B982" s="0" t="s">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" s="0" t="s">
+        <v>1964</v>
+      </c>
+      <c r="B983" s="0" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" s="0" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B984" s="0" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" s="0" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B985" s="0" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" s="0" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B986" s="0" t="s">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" s="0" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B987" s="0" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" s="0" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B988" s="0" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" s="0" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B989" s="0" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" s="0" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B990" s="0" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" s="0" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B991" s="0" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" s="0" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B992" s="0" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" s="0" t="s">
+        <v>1984</v>
+      </c>
+      <c r="B993" s="0" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" s="0" t="s">
+        <v>1986</v>
+      </c>
+      <c r="B994" s="0" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" s="0" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B995" s="0" t="s">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" s="0" t="s">
+        <v>1990</v>
+      </c>
+      <c r="B996" s="0" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" s="0" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B997" s="0" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" s="0" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B998" s="0" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" s="0" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B999" s="0" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="0" t="s">
+        <v>1998</v>
+      </c>
+      <c r="B1000" s="0" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="0" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1001" s="0" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" s="0" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B1002" s="0" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="0" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B1003" s="0" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="0" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B1004" s="0" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="0" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B1005" s="0" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="0" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B1006" s="0" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="0" t="s">
+        <v>2012</v>
+      </c>
+      <c r="B1007" s="0" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" s="0" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B1008" s="0" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" s="0" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B1009" s="0" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="0" t="s">
+        <v>2018</v>
+      </c>
+      <c r="B1010" s="0" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" s="0" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B1011" s="0" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" s="0" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B1012" s="0" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="0" t="s">
+        <v>2024</v>
+      </c>
+      <c r="B1013" s="0" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="0" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B1014" s="0" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" s="0" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B1015" s="0" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" s="0" t="s">
+        <v>2030</v>
+      </c>
+      <c r="B1016" s="0" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" s="0" t="s">
+        <v>2032</v>
+      </c>
+      <c r="B1017" s="0" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" s="0" t="s">
+        <v>2034</v>
+      </c>
+      <c r="B1018" s="0" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" s="0" t="s">
+        <v>2036</v>
+      </c>
+      <c r="B1019" s="0" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" s="0" t="s">
+        <v>2038</v>
+      </c>
+      <c r="B1020" s="0" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" s="0" t="s">
+        <v>2040</v>
+      </c>
+      <c r="B1021" s="0" t="s">
+        <v>2041</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nice titles for registration and deviation graphs. Some text probably too small. Will need to change.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="2042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="2426">
   <si>
     <t>GUID</t>
   </si>
@@ -6162,6 +6162,1158 @@
   </si>
   <si>
     <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 05-Jul-2023 22:18:52</t>
+  </si>
+  <si>
+    <t>001020</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session02_SmoothBatonPosition - 11B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp11B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_11B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 17:52:09</t>
+  </si>
+  <si>
+    <t>001021</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session02_SmoothBatonPosition - 12A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 17:52:27</t>
+  </si>
+  <si>
+    <t>001022</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session02_SmoothBatonPosition - 12A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 17:52:54</t>
+  </si>
+  <si>
+    <t>001023</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session02_SmoothBatonPosition - 12A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp12A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_12A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 18:06:35</t>
+  </si>
+  <si>
+    <t>001024</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session02_SmoothBatonPosition - 51A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp51A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_51A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 18:06:49</t>
+  </si>
+  <si>
+    <t>001025</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session02_SmoothBatonPosition - 51B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp51B_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_51B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 18:07:01</t>
+  </si>
+  <si>
+    <t>001026</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session02_SmoothBatonPosition - 53A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp53A_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_53A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 18:08:38</t>
+  </si>
+  <si>
+    <t>001027</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session02_SmoothBatonPosition - 53C - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session02_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session02_Exp53C_BBaton_etc. data: Session02_SmoothBatonPosition/SavedCycles_Resampled/Smooth_Baton_Pos_53C. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 18:10:17</t>
+  </si>
+  <si>
+    <t>001028</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session03_SmoothBatonPosition and Motive - 42A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp42A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_42A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 19:01:20</t>
+  </si>
+  <si>
+    <t>001029</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session03_SmoothBatonPosition and Motive - 41A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp41A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_41A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 19:01:30</t>
+  </si>
+  <si>
+    <t>001030</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session03_SmoothBatonPosition and Motive - 41A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp41A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_41A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 19:01:55</t>
+  </si>
+  <si>
+    <t>001031</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session03_SmoothBatonPosition and Motive - 41C - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp41C_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_41C. File Location: Visualisations/CalibrationAnalysis. Date Generated: 08-Jul-2023 19:02:05</t>
+  </si>
+  <si>
+    <t>001032</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session03_SmoothBatonPosition and Motive - 51A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 09-Jul-2023 14:12:28</t>
+  </si>
+  <si>
+    <t>001033</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session03_SmoothBatonPosition and Motive - 51B - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51B_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 09-Jul-2023 14:12:32</t>
+  </si>
+  <si>
+    <t>001034</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:38:32</t>
+  </si>
+  <si>
+    <t>001035</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:40:56</t>
+  </si>
+  <si>
+    <t>001036</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:41:43</t>
+  </si>
+  <si>
+    <t>001037</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:42:37</t>
+  </si>
+  <si>
+    <t>001038</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:42:45</t>
+  </si>
+  <si>
+    <t>001039</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:42:58</t>
+  </si>
+  <si>
+    <t>001040</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:44:56</t>
+  </si>
+  <si>
+    <t>001041</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:45:21</t>
+  </si>
+  <si>
+    <t>001042</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:45:51</t>
+  </si>
+  <si>
+    <t>001043</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:46:02</t>
+  </si>
+  <si>
+    <t>001044</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:46:14</t>
+  </si>
+  <si>
+    <t>001045</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:46:24</t>
+  </si>
+  <si>
+    <t>001046</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:47:52</t>
+  </si>
+  <si>
+    <t>001047</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:47:58</t>
+  </si>
+  <si>
+    <t>001048</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:48:09</t>
+  </si>
+  <si>
+    <t>001049</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:49:06</t>
+  </si>
+  <si>
+    <t>001050</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:49:16</t>
+  </si>
+  <si>
+    <t>001051</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:50:04</t>
+  </si>
+  <si>
+    <t>001052</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:50:16</t>
+  </si>
+  <si>
+    <t>001053</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:50:26</t>
+  </si>
+  <si>
+    <t>001054</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 15:53:03</t>
+  </si>
+  <si>
+    <t>001055</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:00:37</t>
+  </si>
+  <si>
+    <t>001056</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:01:24</t>
+  </si>
+  <si>
+    <t>001057</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:05:46</t>
+  </si>
+  <si>
+    <t>001058</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:06:12</t>
+  </si>
+  <si>
+    <t>001059</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:06:20</t>
+  </si>
+  <si>
+    <t>001060</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:06:58</t>
+  </si>
+  <si>
+    <t>001061</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:07:37</t>
+  </si>
+  <si>
+    <t>001062</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:09:34</t>
+  </si>
+  <si>
+    <t>001063</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:10:02</t>
+  </si>
+  <si>
+    <t>001064</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:10:27</t>
+  </si>
+  <si>
+    <t>001065</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:11:29</t>
+  </si>
+  <si>
+    <t>001066</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:11:48</t>
+  </si>
+  <si>
+    <t>001067</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:12:04</t>
+  </si>
+  <si>
+    <t>001068</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:12:48</t>
+  </si>
+  <si>
+    <t>001069</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration + Scaling - Session01_ManipulatedData - Euclidean distance underneath. Arrays shifted to start at highest point.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:13:00</t>
+  </si>
+  <si>
+    <t>001070</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:13:53</t>
+  </si>
+  <si>
+    <t>001071</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:14:01</t>
+  </si>
+  <si>
+    <t>001072</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:14:29</t>
+  </si>
+  <si>
+    <t>001073</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:14:57</t>
+  </si>
+  <si>
+    <t>001074</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:15:21</t>
+  </si>
+  <si>
+    <t>001075</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:15:43</t>
+  </si>
+  <si>
+    <t>001076</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:17:03</t>
+  </si>
+  <si>
+    <t>001077</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:17:42</t>
+  </si>
+  <si>
+    <t>001078</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:17:52</t>
+  </si>
+  <si>
+    <t>001079</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:17:59</t>
+  </si>
+  <si>
+    <t>001080</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:18:43</t>
+  </si>
+  <si>
+    <t>001081</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:18:58</t>
+  </si>
+  <si>
+    <t>001082</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:19:21</t>
+  </si>
+  <si>
+    <t>001083</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:19:45</t>
+  </si>
+  <si>
+    <t>001084</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:19:54</t>
+  </si>
+  <si>
+    <t>001085</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:20:10</t>
+  </si>
+  <si>
+    <t>001086</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:28:17</t>
+  </si>
+  <si>
+    <t>001087</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:28:25</t>
+  </si>
+  <si>
+    <t>001088</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:29:24</t>
+  </si>
+  <si>
+    <t>001089</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:29:33</t>
+  </si>
+  <si>
+    <t>001090</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:29:43</t>
+  </si>
+  <si>
+    <t>001091</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:29:55</t>
+  </si>
+  <si>
+    <t>001092</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:30:17</t>
+  </si>
+  <si>
+    <t>001093</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:36:36</t>
+  </si>
+  <si>
+    <t>001094</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:36:57</t>
+  </si>
+  <si>
+    <t>001095</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:37:23</t>
+  </si>
+  <si>
+    <t>001096</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:38:14</t>
+  </si>
+  <si>
+    <t>001097</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:38:25</t>
+  </si>
+  <si>
+    <t>001098</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:40:01</t>
+  </si>
+  <si>
+    <t>001099</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:40:12</t>
+  </si>
+  <si>
+    <t>001100</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:40:20</t>
+  </si>
+  <si>
+    <t>001101</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:40:34</t>
+  </si>
+  <si>
+    <t>001102</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:41:10</t>
+  </si>
+  <si>
+    <t>001103</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:41:42</t>
+  </si>
+  <si>
+    <t>001104</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:42:09</t>
+  </si>
+  <si>
+    <t>001105</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:42:49</t>
+  </si>
+  <si>
+    <t>001106</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:43:35</t>
+  </si>
+  <si>
+    <t>001107</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:43:49</t>
+  </si>
+  <si>
+    <t>001108</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:44:10</t>
+  </si>
+  <si>
+    <t>001109</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:44:21</t>
+  </si>
+  <si>
+    <t>001110</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:44:46</t>
+  </si>
+  <si>
+    <t>001111</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:44:46</t>
+  </si>
+  <si>
+    <t>001112</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:44:46</t>
+  </si>
+  <si>
+    <t>001113</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:44:46</t>
+  </si>
+  <si>
+    <t>001114</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:44:46</t>
+  </si>
+  <si>
+    <t>001115</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:44:46</t>
+  </si>
+  <si>
+    <t>001116</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:44:46</t>
+  </si>
+  <si>
+    <t>001117</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:45:59</t>
+  </si>
+  <si>
+    <t>001118</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:05</t>
+  </si>
+  <si>
+    <t>001119</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:11</t>
+  </si>
+  <si>
+    <t>001120</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:21</t>
+  </si>
+  <si>
+    <t>001121</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:38</t>
+  </si>
+  <si>
+    <t>001122</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:38</t>
+  </si>
+  <si>
+    <t>001123</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:38</t>
+  </si>
+  <si>
+    <t>001124</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:38</t>
+  </si>
+  <si>
+    <t>001125</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:38</t>
+  </si>
+  <si>
+    <t>001126</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:38</t>
+  </si>
+  <si>
+    <t>001127</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:46:38</t>
+  </si>
+  <si>
+    <t>001128</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:10</t>
+  </si>
+  <si>
+    <t>001129</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:10</t>
+  </si>
+  <si>
+    <t>001130</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:10</t>
+  </si>
+  <si>
+    <t>001131</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:10</t>
+  </si>
+  <si>
+    <t>001132</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:10</t>
+  </si>
+  <si>
+    <t>001133</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:10</t>
+  </si>
+  <si>
+    <t>001134</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:10</t>
+  </si>
+  <si>
+    <t>001135</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:43</t>
+  </si>
+  <si>
+    <t>001136</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:43</t>
+  </si>
+  <si>
+    <t>001137</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:43</t>
+  </si>
+  <si>
+    <t>001138</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:43</t>
+  </si>
+  <si>
+    <t>001139</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:43</t>
+  </si>
+  <si>
+    <t>001140</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:43</t>
+  </si>
+  <si>
+    <t>001141</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp C1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:43</t>
+  </si>
+  <si>
+    <t>001142</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:55</t>
+  </si>
+  <si>
+    <t>001143</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:55</t>
+  </si>
+  <si>
+    <t>001144</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:55</t>
+  </si>
+  <si>
+    <t>001145</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:55</t>
+  </si>
+  <si>
+    <t>001146</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:55</t>
+  </si>
+  <si>
+    <t>001147</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:55</t>
+  </si>
+  <si>
+    <t>001148</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:47:55</t>
+  </si>
+  <si>
+    <t>001149</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 003 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:48:18</t>
+  </si>
+  <si>
+    <t>001150</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 006 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:48:23</t>
+  </si>
+  <si>
+    <t>001151</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:48:29</t>
+  </si>
+  <si>
+    <t>001152</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:48:36</t>
+  </si>
+  <si>
+    <t>001153</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:49:05</t>
+  </si>
+  <si>
+    <t>001154</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:49:05</t>
+  </si>
+  <si>
+    <t>001155</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:49:05</t>
+  </si>
+  <si>
+    <t>001156</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:49:05</t>
+  </si>
+  <si>
+    <t>001157</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:49:05</t>
+  </si>
+  <si>
+    <t>001158</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:49:05</t>
+  </si>
+  <si>
+    <t>001159</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:49:05</t>
+  </si>
+  <si>
+    <t>001160</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:49:40</t>
+  </si>
+  <si>
+    <t>001161</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:49:46</t>
+  </si>
+  <si>
+    <t>001162</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:50:00</t>
+  </si>
+  <si>
+    <t>001163</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:50:26</t>
+  </si>
+  <si>
+    <t>001164</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:50:43</t>
+  </si>
+  <si>
+    <t>001165</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:50:43</t>
+  </si>
+  <si>
+    <t>001166</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:50:43</t>
+  </si>
+  <si>
+    <t>001167</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:50:43</t>
+  </si>
+  <si>
+    <t>001168</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:50:43</t>
+  </si>
+  <si>
+    <t>001169</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:50:43</t>
+  </si>
+  <si>
+    <t>001170</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp D1 002 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:50:43</t>
+  </si>
+  <si>
+    <t>001171</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:51:07</t>
+  </si>
+  <si>
+    <t>001172</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:51:15</t>
+  </si>
+  <si>
+    <t>001173</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:51:31</t>
+  </si>
+  <si>
+    <t>001174</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:51:38</t>
+  </si>
+  <si>
+    <t>001175</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:51:44</t>
+  </si>
+  <si>
+    <t>001176</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 5. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:51:52</t>
+  </si>
+  <si>
+    <t>001177</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:51:58</t>
+  </si>
+  <si>
+    <t>001178</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:05</t>
+  </si>
+  <si>
+    <t>001179</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:17</t>
+  </si>
+  <si>
+    <t>001180</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:17</t>
+  </si>
+  <si>
+    <t>001181</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:17</t>
+  </si>
+  <si>
+    <t>001182</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:17</t>
+  </si>
+  <si>
+    <t>001183</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:17</t>
+  </si>
+  <si>
+    <t>001184</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:17</t>
+  </si>
+  <si>
+    <t>001185</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp E1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:17</t>
+  </si>
+  <si>
+    <t>001186</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 1. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:51</t>
+  </si>
+  <si>
+    <t>001187</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 4. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:52:59</t>
+  </si>
+  <si>
+    <t>001188</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:07</t>
+  </si>
+  <si>
+    <t>001189</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:12</t>
+  </si>
+  <si>
+    <t>001190</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:22</t>
+  </si>
+  <si>
+    <t>001191</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:36</t>
+  </si>
+  <si>
+    <t>001192</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:46</t>
+  </si>
+  <si>
+    <t>001193</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:54</t>
+  </si>
+  <si>
+    <t>001194</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:54</t>
+  </si>
+  <si>
+    <t>001195</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:54</t>
+  </si>
+  <si>
+    <t>001196</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:54</t>
+  </si>
+  <si>
+    <t>001197</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:54</t>
+  </si>
+  <si>
+    <t>001198</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:54</t>
+  </si>
+  <si>
+    <t>001199</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 16:53:54</t>
+  </si>
+  <si>
+    <t>001200</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:05:36</t>
+  </si>
+  <si>
+    <t>001201</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp F1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:05:36</t>
+  </si>
+  <si>
+    <t>001202</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp F1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:07:07</t>
+  </si>
+  <si>
+    <t>001203</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp F1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:07:07</t>
+  </si>
+  <si>
+    <t>001204</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp B1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:08:01</t>
+  </si>
+  <si>
+    <t>001205</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp B1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:08:01</t>
+  </si>
+  <si>
+    <t>001206</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp C1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:08:23</t>
+  </si>
+  <si>
+    <t>001207</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp C1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:08:23</t>
+  </si>
+  <si>
+    <t>001208</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp D1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:08:44</t>
+  </si>
+  <si>
+    <t>001209</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp D1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:08:44</t>
+  </si>
+  <si>
+    <t>001210</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp E1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:09:47</t>
+  </si>
+  <si>
+    <t>001211</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation.. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp E1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 17:09:47</t>
   </si>
 </sst>
 </file>
@@ -6531,7 +7683,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B1021"/>
+  <dimension ref="A1:B1213"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -14711,6 +15863,1542 @@
         <v>2041</v>
       </c>
     </row>
+    <row r="1022">
+      <c r="A1022" s="0" t="s">
+        <v>2042</v>
+      </c>
+      <c r="B1022" s="0" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" s="0" t="s">
+        <v>2044</v>
+      </c>
+      <c r="B1023" s="0" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" s="0" t="s">
+        <v>2046</v>
+      </c>
+      <c r="B1024" s="0" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" s="0" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B1025" s="0" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" s="0" t="s">
+        <v>2050</v>
+      </c>
+      <c r="B1026" s="0" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" s="0" t="s">
+        <v>2052</v>
+      </c>
+      <c r="B1027" s="0" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" s="0" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1028" s="0" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" s="0" t="s">
+        <v>2056</v>
+      </c>
+      <c r="B1029" s="0" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" s="0" t="s">
+        <v>2058</v>
+      </c>
+      <c r="B1030" s="0" t="s">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" s="0" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B1031" s="0" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" s="0" t="s">
+        <v>2062</v>
+      </c>
+      <c r="B1032" s="0" t="s">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" s="0" t="s">
+        <v>2064</v>
+      </c>
+      <c r="B1033" s="0" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" s="0" t="s">
+        <v>2066</v>
+      </c>
+      <c r="B1034" s="0" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" s="0" t="s">
+        <v>2068</v>
+      </c>
+      <c r="B1035" s="0" t="s">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" s="0" t="s">
+        <v>2070</v>
+      </c>
+      <c r="B1036" s="0" t="s">
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" s="0" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B1037" s="0" t="s">
+        <v>2073</v>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" s="0" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B1038" s="0" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" s="0" t="s">
+        <v>2076</v>
+      </c>
+      <c r="B1039" s="0" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" s="0" t="s">
+        <v>2078</v>
+      </c>
+      <c r="B1040" s="0" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" s="0" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B1041" s="0" t="s">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" s="0" t="s">
+        <v>2082</v>
+      </c>
+      <c r="B1042" s="0" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" s="0" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B1043" s="0" t="s">
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" s="0" t="s">
+        <v>2086</v>
+      </c>
+      <c r="B1044" s="0" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" s="0" t="s">
+        <v>2088</v>
+      </c>
+      <c r="B1045" s="0" t="s">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" s="0" t="s">
+        <v>2090</v>
+      </c>
+      <c r="B1046" s="0" t="s">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" s="0" t="s">
+        <v>2092</v>
+      </c>
+      <c r="B1047" s="0" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" s="0" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B1048" s="0" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" s="0" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B1049" s="0" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" s="0" t="s">
+        <v>2098</v>
+      </c>
+      <c r="B1050" s="0" t="s">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" s="0" t="s">
+        <v>2100</v>
+      </c>
+      <c r="B1051" s="0" t="s">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" s="0" t="s">
+        <v>2102</v>
+      </c>
+      <c r="B1052" s="0" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" s="0" t="s">
+        <v>2104</v>
+      </c>
+      <c r="B1053" s="0" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" s="0" t="s">
+        <v>2106</v>
+      </c>
+      <c r="B1054" s="0" t="s">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" s="0" t="s">
+        <v>2108</v>
+      </c>
+      <c r="B1055" s="0" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" s="0" t="s">
+        <v>2110</v>
+      </c>
+      <c r="B1056" s="0" t="s">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" s="0" t="s">
+        <v>2112</v>
+      </c>
+      <c r="B1057" s="0" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" s="0" t="s">
+        <v>2114</v>
+      </c>
+      <c r="B1058" s="0" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" s="0" t="s">
+        <v>2116</v>
+      </c>
+      <c r="B1059" s="0" t="s">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" s="0" t="s">
+        <v>2118</v>
+      </c>
+      <c r="B1060" s="0" t="s">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" s="0" t="s">
+        <v>2120</v>
+      </c>
+      <c r="B1061" s="0" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" s="0" t="s">
+        <v>2122</v>
+      </c>
+      <c r="B1062" s="0" t="s">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" s="0" t="s">
+        <v>2124</v>
+      </c>
+      <c r="B1063" s="0" t="s">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" s="0" t="s">
+        <v>2126</v>
+      </c>
+      <c r="B1064" s="0" t="s">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" s="0" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B1065" s="0" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" s="0" t="s">
+        <v>2130</v>
+      </c>
+      <c r="B1066" s="0" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" s="0" t="s">
+        <v>2132</v>
+      </c>
+      <c r="B1067" s="0" t="s">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" s="0" t="s">
+        <v>2134</v>
+      </c>
+      <c r="B1068" s="0" t="s">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" s="0" t="s">
+        <v>2136</v>
+      </c>
+      <c r="B1069" s="0" t="s">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" s="0" t="s">
+        <v>2138</v>
+      </c>
+      <c r="B1070" s="0" t="s">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" s="0" t="s">
+        <v>2140</v>
+      </c>
+      <c r="B1071" s="0" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" s="0" t="s">
+        <v>2142</v>
+      </c>
+      <c r="B1072" s="0" t="s">
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" s="0" t="s">
+        <v>2144</v>
+      </c>
+      <c r="B1073" s="0" t="s">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" s="0" t="s">
+        <v>2146</v>
+      </c>
+      <c r="B1074" s="0" t="s">
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" s="0" t="s">
+        <v>2148</v>
+      </c>
+      <c r="B1075" s="0" t="s">
+        <v>2149</v>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" s="0" t="s">
+        <v>2150</v>
+      </c>
+      <c r="B1076" s="0" t="s">
+        <v>2151</v>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" s="0" t="s">
+        <v>2152</v>
+      </c>
+      <c r="B1077" s="0" t="s">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" s="0" t="s">
+        <v>2154</v>
+      </c>
+      <c r="B1078" s="0" t="s">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" s="0" t="s">
+        <v>2156</v>
+      </c>
+      <c r="B1079" s="0" t="s">
+        <v>2157</v>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" s="0" t="s">
+        <v>2158</v>
+      </c>
+      <c r="B1080" s="0" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" s="0" t="s">
+        <v>2160</v>
+      </c>
+      <c r="B1081" s="0" t="s">
+        <v>2161</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" s="0" t="s">
+        <v>2162</v>
+      </c>
+      <c r="B1082" s="0" t="s">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" s="0" t="s">
+        <v>2164</v>
+      </c>
+      <c r="B1083" s="0" t="s">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" s="0" t="s">
+        <v>2166</v>
+      </c>
+      <c r="B1084" s="0" t="s">
+        <v>2167</v>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" s="0" t="s">
+        <v>2168</v>
+      </c>
+      <c r="B1085" s="0" t="s">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" s="0" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B1086" s="0" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" s="0" t="s">
+        <v>2172</v>
+      </c>
+      <c r="B1087" s="0" t="s">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" s="0" t="s">
+        <v>2174</v>
+      </c>
+      <c r="B1088" s="0" t="s">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" s="0" t="s">
+        <v>2176</v>
+      </c>
+      <c r="B1089" s="0" t="s">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" s="0" t="s">
+        <v>2178</v>
+      </c>
+      <c r="B1090" s="0" t="s">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" s="0" t="s">
+        <v>2180</v>
+      </c>
+      <c r="B1091" s="0" t="s">
+        <v>2181</v>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" s="0" t="s">
+        <v>2182</v>
+      </c>
+      <c r="B1092" s="0" t="s">
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" s="0" t="s">
+        <v>2184</v>
+      </c>
+      <c r="B1093" s="0" t="s">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" s="0" t="s">
+        <v>2186</v>
+      </c>
+      <c r="B1094" s="0" t="s">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" s="0" t="s">
+        <v>2188</v>
+      </c>
+      <c r="B1095" s="0" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" s="0" t="s">
+        <v>2190</v>
+      </c>
+      <c r="B1096" s="0" t="s">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" s="0" t="s">
+        <v>2192</v>
+      </c>
+      <c r="B1097" s="0" t="s">
+        <v>2193</v>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" s="0" t="s">
+        <v>2194</v>
+      </c>
+      <c r="B1098" s="0" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" s="0" t="s">
+        <v>2196</v>
+      </c>
+      <c r="B1099" s="0" t="s">
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" s="0" t="s">
+        <v>2198</v>
+      </c>
+      <c r="B1100" s="0" t="s">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" s="0" t="s">
+        <v>2200</v>
+      </c>
+      <c r="B1101" s="0" t="s">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" s="0" t="s">
+        <v>2202</v>
+      </c>
+      <c r="B1102" s="0" t="s">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" s="0" t="s">
+        <v>2204</v>
+      </c>
+      <c r="B1103" s="0" t="s">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" s="0" t="s">
+        <v>2206</v>
+      </c>
+      <c r="B1104" s="0" t="s">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" s="0" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B1105" s="0" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" s="0" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B1106" s="0" t="s">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" s="0" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B1107" s="0" t="s">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" s="0" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B1108" s="0" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" s="0" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B1109" s="0" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" s="0" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B1110" s="0" t="s">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" s="0" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B1111" s="0" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" s="0" t="s">
+        <v>2222</v>
+      </c>
+      <c r="B1112" s="0" t="s">
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" s="0" t="s">
+        <v>2224</v>
+      </c>
+      <c r="B1113" s="0" t="s">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" s="0" t="s">
+        <v>2226</v>
+      </c>
+      <c r="B1114" s="0" t="s">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" s="0" t="s">
+        <v>2228</v>
+      </c>
+      <c r="B1115" s="0" t="s">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" s="0" t="s">
+        <v>2230</v>
+      </c>
+      <c r="B1116" s="0" t="s">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" s="0" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B1117" s="0" t="s">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" s="0" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B1118" s="0" t="s">
+        <v>2235</v>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" s="0" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B1119" s="0" t="s">
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" s="0" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B1120" s="0" t="s">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" s="0" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B1121" s="0" t="s">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" s="0" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B1122" s="0" t="s">
+        <v>2243</v>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" s="0" t="s">
+        <v>2244</v>
+      </c>
+      <c r="B1123" s="0" t="s">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" s="0" t="s">
+        <v>2246</v>
+      </c>
+      <c r="B1124" s="0" t="s">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" s="0" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B1125" s="0" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" s="0" t="s">
+        <v>2250</v>
+      </c>
+      <c r="B1126" s="0" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" s="0" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1127" s="0" t="s">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" s="0" t="s">
+        <v>2254</v>
+      </c>
+      <c r="B1128" s="0" t="s">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" s="0" t="s">
+        <v>2256</v>
+      </c>
+      <c r="B1129" s="0" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" s="0" t="s">
+        <v>2258</v>
+      </c>
+      <c r="B1130" s="0" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" s="0" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B1131" s="0" t="s">
+        <v>2261</v>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" s="0" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B1132" s="0" t="s">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" s="0" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B1133" s="0" t="s">
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" s="0" t="s">
+        <v>2266</v>
+      </c>
+      <c r="B1134" s="0" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" s="0" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B1135" s="0" t="s">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" s="0" t="s">
+        <v>2270</v>
+      </c>
+      <c r="B1136" s="0" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" s="0" t="s">
+        <v>2272</v>
+      </c>
+      <c r="B1137" s="0" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" s="0" t="s">
+        <v>2274</v>
+      </c>
+      <c r="B1138" s="0" t="s">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" s="0" t="s">
+        <v>2276</v>
+      </c>
+      <c r="B1139" s="0" t="s">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" s="0" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B1140" s="0" t="s">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" s="0" t="s">
+        <v>2280</v>
+      </c>
+      <c r="B1141" s="0" t="s">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" s="0" t="s">
+        <v>2282</v>
+      </c>
+      <c r="B1142" s="0" t="s">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" s="0" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B1143" s="0" t="s">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" s="0" t="s">
+        <v>2286</v>
+      </c>
+      <c r="B1144" s="0" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" s="0" t="s">
+        <v>2288</v>
+      </c>
+      <c r="B1145" s="0" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" s="0" t="s">
+        <v>2290</v>
+      </c>
+      <c r="B1146" s="0" t="s">
+        <v>2291</v>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" s="0" t="s">
+        <v>2292</v>
+      </c>
+      <c r="B1147" s="0" t="s">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" s="0" t="s">
+        <v>2294</v>
+      </c>
+      <c r="B1148" s="0" t="s">
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" s="0" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B1149" s="0" t="s">
+        <v>2297</v>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" s="0" t="s">
+        <v>2298</v>
+      </c>
+      <c r="B1150" s="0" t="s">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" s="0" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B1151" s="0" t="s">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" s="0" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B1152" s="0" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" s="0" t="s">
+        <v>2304</v>
+      </c>
+      <c r="B1153" s="0" t="s">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" s="0" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B1154" s="0" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" s="0" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1155" s="0" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" s="0" t="s">
+        <v>2310</v>
+      </c>
+      <c r="B1156" s="0" t="s">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" s="0" t="s">
+        <v>2312</v>
+      </c>
+      <c r="B1157" s="0" t="s">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" s="0" t="s">
+        <v>2314</v>
+      </c>
+      <c r="B1158" s="0" t="s">
+        <v>2315</v>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" s="0" t="s">
+        <v>2316</v>
+      </c>
+      <c r="B1159" s="0" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" s="0" t="s">
+        <v>2318</v>
+      </c>
+      <c r="B1160" s="0" t="s">
+        <v>2319</v>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" s="0" t="s">
+        <v>2320</v>
+      </c>
+      <c r="B1161" s="0" t="s">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" s="0" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B1162" s="0" t="s">
+        <v>2323</v>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" s="0" t="s">
+        <v>2324</v>
+      </c>
+      <c r="B1163" s="0" t="s">
+        <v>2325</v>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" s="0" t="s">
+        <v>2326</v>
+      </c>
+      <c r="B1164" s="0" t="s">
+        <v>2327</v>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" s="0" t="s">
+        <v>2328</v>
+      </c>
+      <c r="B1165" s="0" t="s">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" s="0" t="s">
+        <v>2330</v>
+      </c>
+      <c r="B1166" s="0" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" s="0" t="s">
+        <v>2332</v>
+      </c>
+      <c r="B1167" s="0" t="s">
+        <v>2333</v>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" s="0" t="s">
+        <v>2334</v>
+      </c>
+      <c r="B1168" s="0" t="s">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" s="0" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B1169" s="0" t="s">
+        <v>2337</v>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" s="0" t="s">
+        <v>2338</v>
+      </c>
+      <c r="B1170" s="0" t="s">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" s="0" t="s">
+        <v>2340</v>
+      </c>
+      <c r="B1171" s="0" t="s">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" s="0" t="s">
+        <v>2342</v>
+      </c>
+      <c r="B1172" s="0" t="s">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" s="0" t="s">
+        <v>2344</v>
+      </c>
+      <c r="B1173" s="0" t="s">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" s="0" t="s">
+        <v>2346</v>
+      </c>
+      <c r="B1174" s="0" t="s">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" s="0" t="s">
+        <v>2348</v>
+      </c>
+      <c r="B1175" s="0" t="s">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" s="0" t="s">
+        <v>2350</v>
+      </c>
+      <c r="B1176" s="0" t="s">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" s="0" t="s">
+        <v>2352</v>
+      </c>
+      <c r="B1177" s="0" t="s">
+        <v>2353</v>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" s="0" t="s">
+        <v>2354</v>
+      </c>
+      <c r="B1178" s="0" t="s">
+        <v>2355</v>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" s="0" t="s">
+        <v>2356</v>
+      </c>
+      <c r="B1179" s="0" t="s">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" s="0" t="s">
+        <v>2358</v>
+      </c>
+      <c r="B1180" s="0" t="s">
+        <v>2359</v>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" s="0" t="s">
+        <v>2360</v>
+      </c>
+      <c r="B1181" s="0" t="s">
+        <v>2361</v>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" s="0" t="s">
+        <v>2362</v>
+      </c>
+      <c r="B1182" s="0" t="s">
+        <v>2363</v>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" s="0" t="s">
+        <v>2364</v>
+      </c>
+      <c r="B1183" s="0" t="s">
+        <v>2365</v>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" s="0" t="s">
+        <v>2366</v>
+      </c>
+      <c r="B1184" s="0" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" s="0" t="s">
+        <v>2368</v>
+      </c>
+      <c r="B1185" s="0" t="s">
+        <v>2369</v>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" s="0" t="s">
+        <v>2370</v>
+      </c>
+      <c r="B1186" s="0" t="s">
+        <v>2371</v>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" s="0" t="s">
+        <v>2372</v>
+      </c>
+      <c r="B1187" s="0" t="s">
+        <v>2373</v>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" s="0" t="s">
+        <v>2374</v>
+      </c>
+      <c r="B1188" s="0" t="s">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" s="0" t="s">
+        <v>2376</v>
+      </c>
+      <c r="B1189" s="0" t="s">
+        <v>2377</v>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" s="0" t="s">
+        <v>2378</v>
+      </c>
+      <c r="B1190" s="0" t="s">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" s="0" t="s">
+        <v>2380</v>
+      </c>
+      <c r="B1191" s="0" t="s">
+        <v>2381</v>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" s="0" t="s">
+        <v>2382</v>
+      </c>
+      <c r="B1192" s="0" t="s">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" s="0" t="s">
+        <v>2384</v>
+      </c>
+      <c r="B1193" s="0" t="s">
+        <v>2385</v>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" s="0" t="s">
+        <v>2386</v>
+      </c>
+      <c r="B1194" s="0" t="s">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" s="0" t="s">
+        <v>2388</v>
+      </c>
+      <c r="B1195" s="0" t="s">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" s="0" t="s">
+        <v>2390</v>
+      </c>
+      <c r="B1196" s="0" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" s="0" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B1197" s="0" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" s="0" t="s">
+        <v>2394</v>
+      </c>
+      <c r="B1198" s="0" t="s">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" s="0" t="s">
+        <v>2396</v>
+      </c>
+      <c r="B1199" s="0" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" s="0" t="s">
+        <v>2398</v>
+      </c>
+      <c r="B1200" s="0" t="s">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" s="0" t="s">
+        <v>2400</v>
+      </c>
+      <c r="B1201" s="0" t="s">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" s="0" t="s">
+        <v>2402</v>
+      </c>
+      <c r="B1202" s="0" t="s">
+        <v>2403</v>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" s="0" t="s">
+        <v>2404</v>
+      </c>
+      <c r="B1203" s="0" t="s">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" s="0" t="s">
+        <v>2406</v>
+      </c>
+      <c r="B1204" s="0" t="s">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" s="0" t="s">
+        <v>2408</v>
+      </c>
+      <c r="B1205" s="0" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" s="0" t="s">
+        <v>2410</v>
+      </c>
+      <c r="B1206" s="0" t="s">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" s="0" t="s">
+        <v>2412</v>
+      </c>
+      <c r="B1207" s="0" t="s">
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" s="0" t="s">
+        <v>2414</v>
+      </c>
+      <c r="B1208" s="0" t="s">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" s="0" t="s">
+        <v>2416</v>
+      </c>
+      <c r="B1209" s="0" t="s">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" s="0" t="s">
+        <v>2418</v>
+      </c>
+      <c r="B1210" s="0" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" s="0" t="s">
+        <v>2420</v>
+      </c>
+      <c r="B1211" s="0" t="s">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" s="0" t="s">
+        <v>2422</v>
+      </c>
+      <c r="B1212" s="0" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" s="0" t="s">
+        <v>2424</v>
+      </c>
+      <c r="B1213" s="0" t="s">
+        <v>2425</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
system to motive registration. re made graphs for lots of figures.
</commit_message>
<xml_diff>
--- a/GUID_Directory.xlsx
+++ b/GUID_Directory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2554" uniqueCount="2554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="2780">
   <si>
     <t>GUID</t>
   </si>
@@ -7698,6 +7698,684 @@
   </si>
   <si>
     <t>Details: Rigid Registration Scaling and Deviation Extraneous Upper Arm Movement against Control. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp F1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 09-Jul-2023 20:35:48</t>
+  </si>
+  <si>
+    <t>001276</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session03_SmoothBatonPosition and Motive - 51B - Euclidean distance underneath. Script used: CalibrationDeviation_Manual.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51B_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 14:06:44</t>
+  </si>
+  <si>
+    <t>001277</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session03_SmoothBatonPosition and Motive - 51A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 14:06:52</t>
+  </si>
+  <si>
+    <t>001278</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Session03 Calibration - Session03_SmoothBatonPosition and Motive - 51A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 14:07:09</t>
+  </si>
+  <si>
+    <t>001279</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Registration - Session03_SmoothBatonPosition and Motive - 51A - Euclidean distance underneath. Script used: CalibrationDeviation_Registration.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 14:07:21</t>
+  </si>
+  <si>
+    <t>001280</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Registration - Session03_SmoothBatonPosition and Motive - 51B - Euclidean distance underneath. Script used: CalibrationDeviation_Manual.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51B_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 14:07:32</t>
+  </si>
+  <si>
+    <t>001281</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Registration - Session03_SmoothBatonPosition and Motive - 51B - Euclidean distance underneath. Script used: CalibrationDeviation_Manual.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51B_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 15:30:43</t>
+  </si>
+  <si>
+    <t>001282</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Registration - Session03_SmoothBatonPosition and Motive - 51B - Euclidean distance underneath. Script used: CalibrationDeviation_Manual.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51B_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 15:36:51</t>
+  </si>
+  <si>
+    <t>001283</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Registration - Session03_SmoothBatonPosition and Motive - 51A - Euclidean distance underneath. Script used: .  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 15:40:05</t>
+  </si>
+  <si>
+    <t>001284</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Registration - Session03_SmoothBatonPosition and Motive - 51A - Euclidean distance underneath. Script used: .  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 15:41:32</t>
+  </si>
+  <si>
+    <t>001285</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Registration - Session03_SmoothBatonPosition and Motive - 51A - Euclidean distance underneath. Script used: .  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51A_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51A. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 15:42:41</t>
+  </si>
+  <si>
+    <t>001286</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Registration - Session03_SmoothBatonPosition and Motive - 51B - Euclidean distance underneath. Script used: CalibrationDeviation_Manual.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51B_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 15:45:38</t>
+  </si>
+  <si>
+    <t>001287</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Registration - Session03_SmoothBatonPosition and Motive - 51B - Euclidean distance underneath. Script used: CalibrationDeviation_Manual.  Dataset used: reference: Session03_ManipulatedData/TrackingDataTime_Resampled_Scaled_Rotated/Session03_Exp51B_BBaton_etc. data: Session03_SmoothBatonPosition/Smooth_Baton_Pos_51B. File Location: Visualisations/CalibrationAnalysis. Date Generated: 10-Jul-2023 15:45:51</t>
+  </si>
+  <si>
+    <t>001288</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Upper Arm Movement against Control. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp A1 005 SavedCycle 3. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 09:27:02</t>
+  </si>
+  <si>
+    <t>001289</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Upper Arm Movement against Control. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp F1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 10:08:55</t>
+  </si>
+  <si>
+    <t>001290</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Upper Arm Movement against Control. Script used: Averages_RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/led\\Session01 Exp F1 All Resampl. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 10:09:42</t>
+  </si>
+  <si>
+    <t>001291</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:11:00</t>
+  </si>
+  <si>
+    <t>001292</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:11:49</t>
+  </si>
+  <si>
+    <t>001293</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:12:46</t>
+  </si>
+  <si>
+    <t>001294</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:13:36</t>
+  </si>
+  <si>
+    <t>001295</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:14:08</t>
+  </si>
+  <si>
+    <t>001296</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:15:08</t>
+  </si>
+  <si>
+    <t>001297</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:15:46</t>
+  </si>
+  <si>
+    <t>001298</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:16:15</t>
+  </si>
+  <si>
+    <t>001299</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_A1_001_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:20:37</t>
+  </si>
+  <si>
+    <t>001300</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_001_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:20:37</t>
+  </si>
+  <si>
+    <t>001301</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_002_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_002_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:20:38</t>
+  </si>
+  <si>
+    <t>001302</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_003_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_003_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:20:38</t>
+  </si>
+  <si>
+    <t>001303</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_004_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_004_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:20:39</t>
+  </si>
+  <si>
+    <t>001304</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_005_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_005_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:20:39</t>
+  </si>
+  <si>
+    <t>001305</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_001_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_001_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:21:46</t>
+  </si>
+  <si>
+    <t>001306</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_002_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_002_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:22:08</t>
+  </si>
+  <si>
+    <t>001307</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_002_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_002_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:22:13</t>
+  </si>
+  <si>
+    <t>001308</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_003_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_003_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:22:23</t>
+  </si>
+  <si>
+    <t>001309</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_004_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_004_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:22:31</t>
+  </si>
+  <si>
+    <t>001310</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_005_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_005_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:22:37</t>
+  </si>
+  <si>
+    <t>001311</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:31:41</t>
+  </si>
+  <si>
+    <t>001312</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:32:39</t>
+  </si>
+  <si>
+    <t>001313</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:33:21</t>
+  </si>
+  <si>
+    <t>001314</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:34:21</t>
+  </si>
+  <si>
+    <t>001315</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:35:00</t>
+  </si>
+  <si>
+    <t>001316</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_006_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_006_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:35:52</t>
+  </si>
+  <si>
+    <t>001317</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_007_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_007_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:36:18</t>
+  </si>
+  <si>
+    <t>001318</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_008_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_008_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:36:26</t>
+  </si>
+  <si>
+    <t>001319</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:37:56</t>
+  </si>
+  <si>
+    <t>001320</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:39:00</t>
+  </si>
+  <si>
+    <t>001321</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:39:39</t>
+  </si>
+  <si>
+    <t>001322</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:40:18</t>
+  </si>
+  <si>
+    <t>001323</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_009_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_009_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:40:52</t>
+  </si>
+  <si>
+    <t>001324</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:42:24</t>
+  </si>
+  <si>
+    <t>001325</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:43:06</t>
+  </si>
+  <si>
+    <t>001326</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:43:45</t>
+  </si>
+  <si>
+    <t>001327</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:44:26</t>
+  </si>
+  <si>
+    <t>001328</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 11:45:03</t>
+  </si>
+  <si>
+    <t>001329</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_009_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_009_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:45:34</t>
+  </si>
+  <si>
+    <t>001330</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_010_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_010_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:45:42</t>
+  </si>
+  <si>
+    <t>001331</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_011_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_011_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:45:51</t>
+  </si>
+  <si>
+    <t>001332</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_012_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_012_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:46:18</t>
+  </si>
+  <si>
+    <t>001333</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_013_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_013_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 11:46:24</t>
+  </si>
+  <si>
+    <t>001334</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/on Pos B1 011 System SavedCycle 8. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 11:53:26</t>
+  </si>
+  <si>
+    <t>001335</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/on Pos B1 011 System SavedCycle 8. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 11:53:26</t>
+  </si>
+  <si>
+    <t>001336</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/on Pos B1 011 System SavedCycle 8. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 11:53:26</t>
+  </si>
+  <si>
+    <t>001337</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/on Pos B1 011 System SavedCycle 8. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 11:53:26</t>
+  </si>
+  <si>
+    <t>001338</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/on Pos B1 011 System SavedCycle 8. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 11:53:26</t>
+  </si>
+  <si>
+    <t>001339</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/on Pos B1 011 System SavedCycle 8. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 11:53:26</t>
+  </si>
+  <si>
+    <t>001340</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/on Pos B1 011 System SavedCycle 8. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 11:53:26</t>
+  </si>
+  <si>
+    <t>001341</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:31:41</t>
+  </si>
+  <si>
+    <t>001342</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_014_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_014_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:32:00</t>
+  </si>
+  <si>
+    <t>001343</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_014_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_014_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:32:23</t>
+  </si>
+  <si>
+    <t>001344</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:33:32</t>
+  </si>
+  <si>
+    <t>001345</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:34:33</t>
+  </si>
+  <si>
+    <t>001346</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:35:17</t>
+  </si>
+  <si>
+    <t>001347</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:35:57</t>
+  </si>
+  <si>
+    <t>001348</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_015_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_015_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:36:31</t>
+  </si>
+  <si>
+    <t>001349</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_016_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_016_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:36:37</t>
+  </si>
+  <si>
+    <t>001350</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_017_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_017_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:36:45</t>
+  </si>
+  <si>
+    <t>001351</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_018_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_018_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:37:20</t>
+  </si>
+  <si>
+    <t>001352</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:39:25</t>
+  </si>
+  <si>
+    <t>001353</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:40:36</t>
+  </si>
+  <si>
+    <t>001354</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:41:19</t>
+  </si>
+  <si>
+    <t>001355</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:42:00</t>
+  </si>
+  <si>
+    <t>001356</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_And_Save_IMU_And_LeapDevice_System_Data.  Dataset used: Live test data from raw imu reading and raw leap reading. Loop every 20ms, imufilter sample rate 5000. arduino internal delay 200. only plotting last 500 values. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 11-Jul-2023 12:42:38</t>
+  </si>
+  <si>
+    <t>001357</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_019_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_019_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:43:15</t>
+  </si>
+  <si>
+    <t>001358</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_019_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_019_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:43:57</t>
+  </si>
+  <si>
+    <t>001359</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_020_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_020_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:44:05</t>
+  </si>
+  <si>
+    <t>001360</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_021_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_021_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:44:13</t>
+  </si>
+  <si>
+    <t>001361</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_022_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_022_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:44:37</t>
+  </si>
+  <si>
+    <t>001362</t>
+  </si>
+  <si>
+    <t>Details: System_SplitCycles_TimeBased_RelativeTime_Smooth_Baton_Pos_B1_023_System.mat. Script used: Step3_IndividualPathCyclesTimeThreshold.  Dataset used: C:\Users\Courtney\source\repos\ThesisProject\Data\Session04_ManipulatedData\RelativeTime_SystemPos\RelativeTime_Smooth_Baton_Pos_B1_023_System.mat. File Location: Visualisations/Session04_IndividualCyclesTimeThreshold. Date Generated: 11-Jul-2023 12:44:42</t>
+  </si>
+  <si>
+    <t>001363</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:55:01</t>
+  </si>
+  <si>
+    <t>001364</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:55:01</t>
+  </si>
+  <si>
+    <t>001365</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:55:01</t>
+  </si>
+  <si>
+    <t>001366</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:55:01</t>
+  </si>
+  <si>
+    <t>001367</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:55:01</t>
+  </si>
+  <si>
+    <t>001368</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:55:01</t>
+  </si>
+  <si>
+    <t>001369</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation Extraneous Knee Movement against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:55:01</t>
+  </si>
+  <si>
+    <t>001370</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:58:31</t>
+  </si>
+  <si>
+    <t>001371</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:58:31</t>
+  </si>
+  <si>
+    <t>001372</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:58:31</t>
+  </si>
+  <si>
+    <t>001373</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:58:31</t>
+  </si>
+  <si>
+    <t>001374</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:58:31</t>
+  </si>
+  <si>
+    <t>001375</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:58:31</t>
+  </si>
+  <si>
+    <t>001376</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 12:58:31</t>
+  </si>
+  <si>
+    <t>001377</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against No Extraneous Movement (Control). Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:12:45</t>
+  </si>
+  <si>
+    <t>001378</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against No Extraneous Movement (Control). Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:12:45</t>
+  </si>
+  <si>
+    <t>001379</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Knee Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:12:51</t>
+  </si>
+  <si>
+    <t>001380</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Knee Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:12:51</t>
+  </si>
+  <si>
+    <t>001381</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Waist Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:12:56</t>
+  </si>
+  <si>
+    <t>001382</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Waist Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:12:56</t>
+  </si>
+  <si>
+    <t>001383</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Feet Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:12:59</t>
+  </si>
+  <si>
+    <t>001384</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Feet Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:12:59</t>
+  </si>
+  <si>
+    <t>001385</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Wrist Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:13:02</t>
+  </si>
+  <si>
+    <t>001386</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Wrist Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:13:02</t>
+  </si>
+  <si>
+    <t>001387</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:13:07</t>
+  </si>
+  <si>
+    <t>001388</t>
+  </si>
+  <si>
+    <t>Details: Rigid Registration Scaling and Deviation System against Extraneous Upper Arm Movement. Script used: RigidRegistrationAndScalingWithDeviation.  Dataset used: reference: Session01_ManipulatedData/SavedCycles_Resampled/Session01_ExpA1_All_Resampled_Average. data: Session01_ManipulatedData/SavedCycles_Resampled/Session01 Exp B1 001 SavedCycle 2. File Location: Visualisations/RegistrationAnalysis. Date Generated: 11-Jul-2023 13:13:07</t>
   </si>
 </sst>
 </file>
@@ -8067,7 +8745,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5CF72-03EA-4788-9A7F-C78C8D9B9AED}">
-  <dimension ref="A1:B1277"/>
+  <dimension ref="A1:B1390"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -18295,6 +18973,910 @@
         <v>2553</v>
       </c>
     </row>
+    <row r="1278">
+      <c r="A1278" s="0" t="s">
+        <v>2554</v>
+      </c>
+      <c r="B1278" s="0" t="s">
+        <v>2555</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" s="0" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1279" s="0" t="s">
+        <v>2557</v>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" s="0" t="s">
+        <v>2558</v>
+      </c>
+      <c r="B1280" s="0" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" s="0" t="s">
+        <v>2560</v>
+      </c>
+      <c r="B1281" s="0" t="s">
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" s="0" t="s">
+        <v>2562</v>
+      </c>
+      <c r="B1282" s="0" t="s">
+        <v>2563</v>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" s="0" t="s">
+        <v>2564</v>
+      </c>
+      <c r="B1283" s="0" t="s">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" s="0" t="s">
+        <v>2566</v>
+      </c>
+      <c r="B1284" s="0" t="s">
+        <v>2567</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" s="0" t="s">
+        <v>2568</v>
+      </c>
+      <c r="B1285" s="0" t="s">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" s="0" t="s">
+        <v>2570</v>
+      </c>
+      <c r="B1286" s="0" t="s">
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" s="0" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B1287" s="0" t="s">
+        <v>2573</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" s="0" t="s">
+        <v>2574</v>
+      </c>
+      <c r="B1288" s="0" t="s">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" s="0" t="s">
+        <v>2576</v>
+      </c>
+      <c r="B1289" s="0" t="s">
+        <v>2577</v>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" s="0" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B1290" s="0" t="s">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" s="0" t="s">
+        <v>2580</v>
+      </c>
+      <c r="B1291" s="0" t="s">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" s="0" t="s">
+        <v>2582</v>
+      </c>
+      <c r="B1292" s="0" t="s">
+        <v>2583</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" s="0" t="s">
+        <v>2584</v>
+      </c>
+      <c r="B1293" s="0" t="s">
+        <v>2585</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" s="0" t="s">
+        <v>2586</v>
+      </c>
+      <c r="B1294" s="0" t="s">
+        <v>2587</v>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" s="0" t="s">
+        <v>2588</v>
+      </c>
+      <c r="B1295" s="0" t="s">
+        <v>2589</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" s="0" t="s">
+        <v>2590</v>
+      </c>
+      <c r="B1296" s="0" t="s">
+        <v>2591</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" s="0" t="s">
+        <v>2592</v>
+      </c>
+      <c r="B1297" s="0" t="s">
+        <v>2593</v>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" s="0" t="s">
+        <v>2594</v>
+      </c>
+      <c r="B1298" s="0" t="s">
+        <v>2595</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" s="0" t="s">
+        <v>2596</v>
+      </c>
+      <c r="B1299" s="0" t="s">
+        <v>2597</v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" s="0" t="s">
+        <v>2598</v>
+      </c>
+      <c r="B1300" s="0" t="s">
+        <v>2599</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" s="0" t="s">
+        <v>2600</v>
+      </c>
+      <c r="B1301" s="0" t="s">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" s="0" t="s">
+        <v>2602</v>
+      </c>
+      <c r="B1302" s="0" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" s="0" t="s">
+        <v>2604</v>
+      </c>
+      <c r="B1303" s="0" t="s">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" s="0" t="s">
+        <v>2606</v>
+      </c>
+      <c r="B1304" s="0" t="s">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" s="0" t="s">
+        <v>2608</v>
+      </c>
+      <c r="B1305" s="0" t="s">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" s="0" t="s">
+        <v>2610</v>
+      </c>
+      <c r="B1306" s="0" t="s">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" s="0" t="s">
+        <v>2612</v>
+      </c>
+      <c r="B1307" s="0" t="s">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" s="0" t="s">
+        <v>2614</v>
+      </c>
+      <c r="B1308" s="0" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" s="0" t="s">
+        <v>2616</v>
+      </c>
+      <c r="B1309" s="0" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" s="0" t="s">
+        <v>2618</v>
+      </c>
+      <c r="B1310" s="0" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" s="0" t="s">
+        <v>2620</v>
+      </c>
+      <c r="B1311" s="0" t="s">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" s="0" t="s">
+        <v>2622</v>
+      </c>
+      <c r="B1312" s="0" t="s">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" s="0" t="s">
+        <v>2624</v>
+      </c>
+      <c r="B1313" s="0" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" s="0" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B1314" s="0" t="s">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" s="0" t="s">
+        <v>2628</v>
+      </c>
+      <c r="B1315" s="0" t="s">
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" s="0" t="s">
+        <v>2630</v>
+      </c>
+      <c r="B1316" s="0" t="s">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" s="0" t="s">
+        <v>2632</v>
+      </c>
+      <c r="B1317" s="0" t="s">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" s="0" t="s">
+        <v>2634</v>
+      </c>
+      <c r="B1318" s="0" t="s">
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" s="0" t="s">
+        <v>2636</v>
+      </c>
+      <c r="B1319" s="0" t="s">
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" s="0" t="s">
+        <v>2638</v>
+      </c>
+      <c r="B1320" s="0" t="s">
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" s="0" t="s">
+        <v>2640</v>
+      </c>
+      <c r="B1321" s="0" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" s="0" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B1322" s="0" t="s">
+        <v>2643</v>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" s="0" t="s">
+        <v>2644</v>
+      </c>
+      <c r="B1323" s="0" t="s">
+        <v>2645</v>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" s="0" t="s">
+        <v>2646</v>
+      </c>
+      <c r="B1324" s="0" t="s">
+        <v>2647</v>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" s="0" t="s">
+        <v>2648</v>
+      </c>
+      <c r="B1325" s="0" t="s">
+        <v>2649</v>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" s="0" t="s">
+        <v>2650</v>
+      </c>
+      <c r="B1326" s="0" t="s">
+        <v>2651</v>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" s="0" t="s">
+        <v>2652</v>
+      </c>
+      <c r="B1327" s="0" t="s">
+        <v>2653</v>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" s="0" t="s">
+        <v>2654</v>
+      </c>
+      <c r="B1328" s="0" t="s">
+        <v>2655</v>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" s="0" t="s">
+        <v>2656</v>
+      </c>
+      <c r="B1329" s="0" t="s">
+        <v>2657</v>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" s="0" t="s">
+        <v>2658</v>
+      </c>
+      <c r="B1330" s="0" t="s">
+        <v>2659</v>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" s="0" t="s">
+        <v>2660</v>
+      </c>
+      <c r="B1331" s="0" t="s">
+        <v>2661</v>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" s="0" t="s">
+        <v>2662</v>
+      </c>
+      <c r="B1332" s="0" t="s">
+        <v>2663</v>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" s="0" t="s">
+        <v>2664</v>
+      </c>
+      <c r="B1333" s="0" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" s="0" t="s">
+        <v>2666</v>
+      </c>
+      <c r="B1334" s="0" t="s">
+        <v>2667</v>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" s="0" t="s">
+        <v>2668</v>
+      </c>
+      <c r="B1335" s="0" t="s">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" s="0" t="s">
+        <v>2670</v>
+      </c>
+      <c r="B1336" s="0" t="s">
+        <v>2671</v>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" s="0" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B1337" s="0" t="s">
+        <v>2673</v>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" s="0" t="s">
+        <v>2674</v>
+      </c>
+      <c r="B1338" s="0" t="s">
+        <v>2675</v>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" s="0" t="s">
+        <v>2676</v>
+      </c>
+      <c r="B1339" s="0" t="s">
+        <v>2677</v>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" s="0" t="s">
+        <v>2678</v>
+      </c>
+      <c r="B1340" s="0" t="s">
+        <v>2679</v>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" s="0" t="s">
+        <v>2680</v>
+      </c>
+      <c r="B1341" s="0" t="s">
+        <v>2681</v>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" s="0" t="s">
+        <v>2682</v>
+      </c>
+      <c r="B1342" s="0" t="s">
+        <v>2683</v>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" s="0" t="s">
+        <v>2684</v>
+      </c>
+      <c r="B1343" s="0" t="s">
+        <v>2685</v>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" s="0" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B1344" s="0" t="s">
+        <v>2687</v>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" s="0" t="s">
+        <v>2688</v>
+      </c>
+      <c r="B1345" s="0" t="s">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" s="0" t="s">
+        <v>2690</v>
+      </c>
+      <c r="B1346" s="0" t="s">
+        <v>2691</v>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" s="0" t="s">
+        <v>2692</v>
+      </c>
+      <c r="B1347" s="0" t="s">
+        <v>2693</v>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" s="0" t="s">
+        <v>2694</v>
+      </c>
+      <c r="B1348" s="0" t="s">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" s="0" t="s">
+        <v>2696</v>
+      </c>
+      <c r="B1349" s="0" t="s">
+        <v>2697</v>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" s="0" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B1350" s="0" t="s">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" s="0" t="s">
+        <v>2700</v>
+      </c>
+      <c r="B1351" s="0" t="s">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" s="0" t="s">
+        <v>2702</v>
+      </c>
+      <c r="B1352" s="0" t="s">
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" s="0" t="s">
+        <v>2704</v>
+      </c>
+      <c r="B1353" s="0" t="s">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" s="0" t="s">
+        <v>2706</v>
+      </c>
+      <c r="B1354" s="0" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" s="0" t="s">
+        <v>2708</v>
+      </c>
+      <c r="B1355" s="0" t="s">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" s="0" t="s">
+        <v>2710</v>
+      </c>
+      <c r="B1356" s="0" t="s">
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" s="0" t="s">
+        <v>2712</v>
+      </c>
+      <c r="B1357" s="0" t="s">
+        <v>2713</v>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" s="0" t="s">
+        <v>2714</v>
+      </c>
+      <c r="B1358" s="0" t="s">
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" s="0" t="s">
+        <v>2716</v>
+      </c>
+      <c r="B1359" s="0" t="s">
+        <v>2717</v>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" s="0" t="s">
+        <v>2718</v>
+      </c>
+      <c r="B1360" s="0" t="s">
+        <v>2719</v>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" s="0" t="s">
+        <v>2720</v>
+      </c>
+      <c r="B1361" s="0" t="s">
+        <v>2721</v>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" s="0" t="s">
+        <v>2722</v>
+      </c>
+      <c r="B1362" s="0" t="s">
+        <v>2723</v>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" s="0" t="s">
+        <v>2724</v>
+      </c>
+      <c r="B1363" s="0" t="s">
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" s="0" t="s">
+        <v>2726</v>
+      </c>
+      <c r="B1364" s="0" t="s">
+        <v>2727</v>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" s="0" t="s">
+        <v>2728</v>
+      </c>
+      <c r="B1365" s="0" t="s">
+        <v>2729</v>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" s="0" t="s">
+        <v>2730</v>
+      </c>
+      <c r="B1366" s="0" t="s">
+        <v>2731</v>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" s="0" t="s">
+        <v>2732</v>
+      </c>
+      <c r="B1367" s="0" t="s">
+        <v>2733</v>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" s="0" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B1368" s="0" t="s">
+        <v>2735</v>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" s="0" t="s">
+        <v>2736</v>
+      </c>
+      <c r="B1369" s="0" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" s="0" t="s">
+        <v>2738</v>
+      </c>
+      <c r="B1370" s="0" t="s">
+        <v>2739</v>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" s="0" t="s">
+        <v>2740</v>
+      </c>
+      <c r="B1371" s="0" t="s">
+        <v>2741</v>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" s="0" t="s">
+        <v>2742</v>
+      </c>
+      <c r="B1372" s="0" t="s">
+        <v>2743</v>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" s="0" t="s">
+        <v>2744</v>
+      </c>
+      <c r="B1373" s="0" t="s">
+        <v>2745</v>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" s="0" t="s">
+        <v>2746</v>
+      </c>
+      <c r="B1374" s="0" t="s">
+        <v>2747</v>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" s="0" t="s">
+        <v>2748</v>
+      </c>
+      <c r="B1375" s="0" t="s">
+        <v>2749</v>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" s="0" t="s">
+        <v>2750</v>
+      </c>
+      <c r="B1376" s="0" t="s">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" s="0" t="s">
+        <v>2752</v>
+      </c>
+      <c r="B1377" s="0" t="s">
+        <v>2753</v>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" s="0" t="s">
+        <v>2754</v>
+      </c>
+      <c r="B1378" s="0" t="s">
+        <v>2755</v>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" s="0" t="s">
+        <v>2756</v>
+      </c>
+      <c r="B1379" s="0" t="s">
+        <v>2757</v>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" s="0" t="s">
+        <v>2758</v>
+      </c>
+      <c r="B1380" s="0" t="s">
+        <v>2759</v>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" s="0" t="s">
+        <v>2760</v>
+      </c>
+      <c r="B1381" s="0" t="s">
+        <v>2761</v>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" s="0" t="s">
+        <v>2762</v>
+      </c>
+      <c r="B1382" s="0" t="s">
+        <v>2763</v>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" s="0" t="s">
+        <v>2764</v>
+      </c>
+      <c r="B1383" s="0" t="s">
+        <v>2765</v>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" s="0" t="s">
+        <v>2766</v>
+      </c>
+      <c r="B1384" s="0" t="s">
+        <v>2767</v>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" s="0" t="s">
+        <v>2768</v>
+      </c>
+      <c r="B1385" s="0" t="s">
+        <v>2769</v>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" s="0" t="s">
+        <v>2770</v>
+      </c>
+      <c r="B1386" s="0" t="s">
+        <v>2771</v>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" s="0" t="s">
+        <v>2772</v>
+      </c>
+      <c r="B1387" s="0" t="s">
+        <v>2773</v>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" s="0" t="s">
+        <v>2774</v>
+      </c>
+      <c r="B1388" s="0" t="s">
+        <v>2775</v>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" s="0" t="s">
+        <v>2776</v>
+      </c>
+      <c r="B1389" s="0" t="s">
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" s="0" t="s">
+        <v>2778</v>
+      </c>
+      <c r="B1390" s="0" t="s">
+        <v>2779</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>